<commit_message>
change xlookup to vlookup
some ppl excel not up to date
</commit_message>
<xml_diff>
--- a/Excel Solver Portfolio Optimization.xlsx
+++ b/Excel Solver Portfolio Optimization.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10812"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manfye pc\Desktop\power BI\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manfyegoh/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C664E255-912A-45B4-94FE-D3CA7DD9B90A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D0DF913-B149-B743-A4E2-94221F6376DA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stock Portfolio (MPT)" sheetId="4" r:id="rId1"/>
@@ -111,9 +111,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -177,14 +175,14 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -5987,7 +5985,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="16" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="11" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
     <cellStyle name="Title" xfId="2" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="18" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="15" builtinId="11" customBuiltin="1"/>
@@ -6012,13 +6010,13 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="d/m/yyyy"/>
+      <numFmt numFmtId="165" formatCode="d/m/yyyy"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="13" formatCode="0%"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="d/m/yyyy"/>
+      <numFmt numFmtId="165" formatCode="d/m/yyyy"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="13" formatCode="0%"/>
@@ -6042,7 +6040,7 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="d/m/yyyy"/>
+      <numFmt numFmtId="165" formatCode="d/m/yyyy"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -6066,7 +6064,7 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="d/m/yyyy"/>
+      <numFmt numFmtId="165" formatCode="d/m/yyyy"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
@@ -6090,7 +6088,7 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="d/m/yyyy"/>
+      <numFmt numFmtId="165" formatCode="d/m/yyyy"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
@@ -6114,7 +6112,7 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="d/m/yyyy"/>
+      <numFmt numFmtId="165" formatCode="d/m/yyyy"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -6135,7 +6133,7 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="d/m/yyyy"/>
+      <numFmt numFmtId="165" formatCode="d/m/yyyy"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -6159,7 +6157,7 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="d/m/yyyy"/>
+      <numFmt numFmtId="165" formatCode="d/m/yyyy"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -6352,7 +6350,7 @@
     <tableColumn id="5" xr3:uid="{8280925B-606A-472E-A96E-8777712F55B9}" uniqueName="5" name="Close*" queryTableFieldId="5" dataDxfId="36"/>
     <tableColumn id="6" xr3:uid="{90EF8E20-E8B6-496F-AA8F-BF43A741EB2B}" uniqueName="6" name="Adj Close**" queryTableFieldId="6" dataDxfId="35"/>
     <tableColumn id="7" xr3:uid="{BDAA6E82-2A73-4946-8E67-77D2773D0F53}" uniqueName="7" name="Volume" queryTableFieldId="7" dataDxfId="34"/>
-    <tableColumn id="8" xr3:uid="{BE5C65D9-9F41-4EFC-A04A-99C9FAC24B86}" uniqueName="8" name="Top Glove" queryTableFieldId="8" dataDxfId="33" dataCellStyle="Percent"/>
+    <tableColumn id="8" xr3:uid="{BE5C65D9-9F41-4EFC-A04A-99C9FAC24B86}" uniqueName="8" name="Top Glove" queryTableFieldId="8" dataDxfId="33"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6369,7 +6367,7 @@
     <tableColumn id="5" xr3:uid="{975EA8E0-4A0E-4840-976F-DA7D69188F2B}" uniqueName="5" name="Close*" queryTableFieldId="5" dataDxfId="28"/>
     <tableColumn id="6" xr3:uid="{C2C98209-7D22-445A-87FA-E26BA18314E8}" uniqueName="6" name="Adj Close**" queryTableFieldId="6" dataDxfId="27"/>
     <tableColumn id="7" xr3:uid="{C014E5EA-91E6-422E-96EC-AD5E752CBB72}" uniqueName="7" name="Volume" queryTableFieldId="7" dataDxfId="26"/>
-    <tableColumn id="8" xr3:uid="{7845321C-1EF8-495A-8FED-400927CB6846}" uniqueName="8" name="SuperMX" queryTableFieldId="8" dataDxfId="25" dataCellStyle="Percent"/>
+    <tableColumn id="8" xr3:uid="{7845321C-1EF8-495A-8FED-400927CB6846}" uniqueName="8" name="SuperMX" queryTableFieldId="8" dataDxfId="25"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6386,7 +6384,7 @@
     <tableColumn id="5" xr3:uid="{FEE48B99-8C28-47CE-A9A0-AFF328D95729}" uniqueName="5" name="Close*" queryTableFieldId="5" dataDxfId="20"/>
     <tableColumn id="6" xr3:uid="{46BF69BF-49B9-420F-8DB0-E009E32B2D03}" uniqueName="6" name="Adj Close**" queryTableFieldId="6" dataDxfId="19"/>
     <tableColumn id="7" xr3:uid="{A72CE2F6-A4F2-4DB7-ACCD-E43000738F31}" uniqueName="7" name="Volume" queryTableFieldId="7" dataDxfId="18"/>
-    <tableColumn id="8" xr3:uid="{AE5E1D2B-D2F1-4E72-9CF1-56217919423D}" uniqueName="8" name="MYEG" queryTableFieldId="8" dataDxfId="17" dataCellStyle="Percent"/>
+    <tableColumn id="8" xr3:uid="{AE5E1D2B-D2F1-4E72-9CF1-56217919423D}" uniqueName="8" name="MYEG" queryTableFieldId="8" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6712,28 +6710,28 @@
   <dimension ref="A1:AB146"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L42" sqref="L42"/>
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" hidden="1" customWidth="1"/>
     <col min="3" max="6" width="12" customWidth="1"/>
-    <col min="8" max="8" width="0" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="29.5703125" customWidth="1"/>
-    <col min="10" max="10" width="21.85546875" customWidth="1"/>
-    <col min="11" max="11" width="14.28515625" customWidth="1"/>
-    <col min="12" max="12" width="30.5703125" customWidth="1"/>
-    <col min="13" max="13" width="11.85546875" customWidth="1"/>
-    <col min="14" max="14" width="9.140625" customWidth="1"/>
-    <col min="15" max="15" width="28.28515625" customWidth="1"/>
-    <col min="16" max="16" width="17.42578125" customWidth="1"/>
-    <col min="17" max="17" width="14.28515625" customWidth="1"/>
-    <col min="18" max="18" width="12.7109375" customWidth="1"/>
+    <col min="8" max="8" width="8.83203125" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="29.5" customWidth="1"/>
+    <col min="10" max="10" width="21.83203125" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" customWidth="1"/>
+    <col min="12" max="12" width="30.5" customWidth="1"/>
+    <col min="13" max="13" width="11.83203125" customWidth="1"/>
+    <col min="14" max="14" width="9.1640625" customWidth="1"/>
+    <col min="15" max="15" width="28.33203125" customWidth="1"/>
+    <col min="16" max="16" width="17.5" customWidth="1"/>
+    <col min="17" max="17" width="14.33203125" customWidth="1"/>
+    <col min="18" max="18" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1" s="32" t="s">
         <v>1210</v>
       </c>
@@ -6763,7 +6761,7 @@
       <c r="AA1" s="22"/>
       <c r="AB1" s="22"/>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
         <v>0</v>
       </c>
@@ -6772,11 +6770,11 @@
       </c>
       <c r="C2" s="15" t="str">
         <f>I5</f>
-        <v>DRB HCOM</v>
+        <v>AIR ASIA</v>
       </c>
       <c r="D2" s="15" t="str">
         <f>I6</f>
-        <v>AIR ASIA</v>
+        <v>DRB HCOM</v>
       </c>
       <c r="E2" s="15" t="str">
         <f>I7</f>
@@ -6813,20 +6811,20 @@
       <c r="AA2" s="22"/>
       <c r="AB2" s="22"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A3" s="28">
         <v>43983</v>
       </c>
       <c r="B3" s="20">
         <v>1</v>
       </c>
-      <c r="C3" s="21" cm="1">
-        <f t="array" aca="1" ref="C3" ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B3+1)</f>
-        <v>4.2424242424242462E-2</v>
+      <c r="C3" s="21">
+        <f ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B3+1)</f>
+        <v>0</v>
       </c>
       <c r="D3" s="21" cm="1">
         <f t="array" aca="1" ref="D3" ca="1">INDIRECT("'Raw Data'!"&amp;$H$4&amp;$B3+1)</f>
-        <v>0</v>
+        <v>4.2424242424242462E-2</v>
       </c>
       <c r="E3" s="21" cm="1">
         <f t="array" aca="1" ref="E3" ca="1">INDIRECT("'Raw Data'!"&amp;$H$5&amp;$B3+1)</f>
@@ -6838,8 +6836,8 @@
       </c>
       <c r="G3" s="22"/>
       <c r="H3" t="str">
-        <f>_xlfn.XLOOKUP(I5,'Stock Selection'!$A$1:$A$8,'Stock Selection'!$B$1:$B$8)</f>
-        <v>BA</v>
+        <f>VLOOKUP('Stock Portfolio (MPT)'!I5,'Stock Selection'!A1:B8,2,FALSE)</f>
+        <v>Q</v>
       </c>
       <c r="I3" s="61"/>
       <c r="J3" s="61"/>
@@ -6862,7 +6860,7 @@
       <c r="AA3" s="22"/>
       <c r="AB3" s="22"/>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A4" s="29">
         <v>43952</v>
       </c>
@@ -6871,11 +6869,11 @@
       </c>
       <c r="C4" s="21" cm="1">
         <f t="array" aca="1" ref="C4" ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B4+1)</f>
-        <v>0.1702127659574468</v>
+        <v>0.28985507246376824</v>
       </c>
       <c r="D4" s="21" cm="1">
         <f t="array" aca="1" ref="D4" ca="1">INDIRECT("'Raw Data'!"&amp;$H$4&amp;$B4+1)</f>
-        <v>0.28985507246376824</v>
+        <v>0.1702127659574468</v>
       </c>
       <c r="E4" s="21" cm="1">
         <f t="array" aca="1" ref="E4" ca="1">INDIRECT("'Raw Data'!"&amp;$H$5&amp;$B4+1)</f>
@@ -6887,8 +6885,8 @@
       </c>
       <c r="G4" s="24"/>
       <c r="H4" t="str">
-        <f>_xlfn.XLOOKUP(I6,'Stock Selection'!$A$1:$A$8,'Stock Selection'!$B$1:$B$8)</f>
-        <v>Q</v>
+        <f>VLOOKUP('Stock Portfolio (MPT)'!I6,'Stock Selection'!A2:B9,2,FALSE)</f>
+        <v>BA</v>
       </c>
       <c r="I4" s="54" t="s">
         <v>1218</v>
@@ -6915,7 +6913,7 @@
       <c r="AA4" s="22"/>
       <c r="AB4" s="22"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A5" s="28">
         <v>43922</v>
       </c>
@@ -6924,11 +6922,11 @@
       </c>
       <c r="C5" s="21" cm="1">
         <f t="array" aca="1" ref="C5" ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B5+1)</f>
-        <v>6.8181818181818066E-2</v>
+        <v>-0.15337423312883436</v>
       </c>
       <c r="D5" s="21" cm="1">
         <f t="array" aca="1" ref="D5" ca="1">INDIRECT("'Raw Data'!"&amp;$H$4&amp;$B5+1)</f>
-        <v>-0.15337423312883436</v>
+        <v>6.8181818181818066E-2</v>
       </c>
       <c r="E5" s="21" cm="1">
         <f t="array" aca="1" ref="E5" ca="1">INDIRECT("'Raw Data'!"&amp;$H$5&amp;$B5+1)</f>
@@ -6940,15 +6938,15 @@
       </c>
       <c r="G5" s="24"/>
       <c r="H5" t="str">
-        <f>_xlfn.XLOOKUP(I7,'Stock Selection'!$A$1:$A$8,'Stock Selection'!$B$1:$B$8)</f>
+        <f>VLOOKUP('Stock Portfolio (MPT)'!I7,'Stock Selection'!A3:B10,2,FALSE)</f>
         <v>AR</v>
       </c>
       <c r="I5" s="13" t="s">
-        <v>1640</v>
+        <v>1645</v>
       </c>
       <c r="J5" s="35" cm="1">
         <f t="array" aca="1" ref="J5" ca="1">AVERAGE(IF(ISERROR(C3:C62),"",C3:C62))</f>
-        <v>1.1844283545269351E-2</v>
+        <v>2.7584808175904904E-2</v>
       </c>
       <c r="K5" s="22"/>
       <c r="L5" s="19"/>
@@ -6969,7 +6967,7 @@
       <c r="AA5" s="22"/>
       <c r="AB5" s="22"/>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A6" s="29">
         <v>43891</v>
       </c>
@@ -6978,11 +6976,11 @@
       </c>
       <c r="C6" s="21" cm="1">
         <f t="array" aca="1" ref="C6" ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B6+1)</f>
-        <v>-0.40540540540540543</v>
+        <v>3.1645569620253049E-2</v>
       </c>
       <c r="D6" s="21" cm="1">
         <f t="array" aca="1" ref="D6" ca="1">INDIRECT("'Raw Data'!"&amp;$H$4&amp;$B6+1)</f>
-        <v>3.1645569620253049E-2</v>
+        <v>-0.40540540540540543</v>
       </c>
       <c r="E6" s="21" cm="1">
         <f t="array" aca="1" ref="E6" ca="1">INDIRECT("'Raw Data'!"&amp;$H$5&amp;$B6+1)</f>
@@ -6994,15 +6992,15 @@
       </c>
       <c r="G6" s="24"/>
       <c r="H6" t="str">
-        <f>_xlfn.XLOOKUP(I8,'Stock Selection'!$A$1:$A$8,'Stock Selection'!$B$1:$B$8)</f>
+        <f>VLOOKUP('Stock Portfolio (MPT)'!I8,'Stock Selection'!A4:B11,2,FALSE)</f>
         <v>Z</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>1645</v>
+        <v>1640</v>
       </c>
       <c r="J6" s="35">
         <f t="array" aca="1" ref="J6" ca="1">AVERAGE(IF(ISERROR(D3:D62),"",D3:D62))</f>
-        <v>2.7584808175904904E-2</v>
+        <v>1.1844283545269351E-2</v>
       </c>
       <c r="K6" s="22"/>
       <c r="L6" s="19"/>
@@ -7023,7 +7021,7 @@
       <c r="AA6" s="22"/>
       <c r="AB6" s="22"/>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A7" s="28">
         <v>43862</v>
       </c>
@@ -7032,11 +7030,11 @@
       </c>
       <c r="C7" s="21" cm="1">
         <f t="array" aca="1" ref="C7" ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B7+1)</f>
-        <v>-2.2026431718061595E-2</v>
+        <v>-0.20999999999999996</v>
       </c>
       <c r="D7" s="21" cm="1">
         <f t="array" aca="1" ref="D7" ca="1">INDIRECT("'Raw Data'!"&amp;$H$4&amp;$B7+1)</f>
-        <v>-0.20999999999999996</v>
+        <v>-2.2026431718061595E-2</v>
       </c>
       <c r="E7" s="21" cm="1">
         <f t="array" aca="1" ref="E7" ca="1">INDIRECT("'Raw Data'!"&amp;$H$5&amp;$B7+1)</f>
@@ -7073,7 +7071,7 @@
       <c r="AA7" s="22"/>
       <c r="AB7" s="22"/>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A8" s="29">
         <v>43831</v>
       </c>
@@ -7082,11 +7080,11 @@
       </c>
       <c r="C8" s="21" cm="1">
         <f t="array" aca="1" ref="C8" ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B8+1)</f>
-        <v>-4.621848739495793E-2</v>
+        <v>-0.30069930069930068</v>
       </c>
       <c r="D8" s="21" cm="1">
         <f t="array" aca="1" ref="D8" ca="1">INDIRECT("'Raw Data'!"&amp;$H$4&amp;$B8+1)</f>
-        <v>-0.30069930069930068</v>
+        <v>-4.621848739495793E-2</v>
       </c>
       <c r="E8" s="21" cm="1">
         <f t="array" aca="1" ref="E8" ca="1">INDIRECT("'Raw Data'!"&amp;$H$5&amp;$B8+1)</f>
@@ -7123,7 +7121,7 @@
       <c r="AA8" s="22"/>
       <c r="AB8" s="22"/>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A9" s="28">
         <v>43800</v>
       </c>
@@ -7132,11 +7130,11 @@
       </c>
       <c r="C9" s="21" cm="1">
         <f t="array" aca="1" ref="C9" ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B9+1)</f>
-        <v>3.0303030303030234E-2</v>
+        <v>-0.15882352941176472</v>
       </c>
       <c r="D9" s="21" cm="1">
         <f t="array" aca="1" ref="D9" ca="1">INDIRECT("'Raw Data'!"&amp;$H$4&amp;$B9+1)</f>
-        <v>-0.15882352941176472</v>
+        <v>3.0303030303030234E-2</v>
       </c>
       <c r="E9" s="21" cm="1">
         <f t="array" aca="1" ref="E9" ca="1">INDIRECT("'Raw Data'!"&amp;$H$5&amp;$B9+1)</f>
@@ -7168,7 +7166,7 @@
       <c r="AA9" s="22"/>
       <c r="AB9" s="22"/>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A10" s="29">
         <v>43770</v>
       </c>
@@ -7177,11 +7175,11 @@
       </c>
       <c r="C10" s="21" cm="1">
         <f t="array" aca="1" ref="C10" ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B10+1)</f>
-        <v>-8.6956521739130349E-2</v>
+        <v>5.9171597633136145E-3</v>
       </c>
       <c r="D10" s="21" cm="1">
         <f t="array" aca="1" ref="D10" ca="1">INDIRECT("'Raw Data'!"&amp;$H$4&amp;$B10+1)</f>
-        <v>5.9171597633136145E-3</v>
+        <v>-8.6956521739130349E-2</v>
       </c>
       <c r="E10" s="21" cm="1">
         <f t="array" aca="1" ref="E10" ca="1">INDIRECT("'Raw Data'!"&amp;$H$5&amp;$B10+1)</f>
@@ -7217,7 +7215,7 @@
       <c r="AA10" s="22"/>
       <c r="AB10" s="22"/>
     </row>
-    <row r="11" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="28">
         <v>43739</v>
       </c>
@@ -7226,11 +7224,11 @@
       </c>
       <c r="C11" s="21" cm="1">
         <f t="array" aca="1" ref="C11" ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B11+1)</f>
-        <v>8.1057984019142743E-2</v>
+        <v>-0.11518324607329843</v>
       </c>
       <c r="D11" s="21" cm="1">
         <f t="array" aca="1" ref="D11" ca="1">INDIRECT("'Raw Data'!"&amp;$H$4&amp;$B11+1)</f>
-        <v>-0.11518324607329843</v>
+        <v>8.1057984019142743E-2</v>
       </c>
       <c r="E11" s="21" cm="1">
         <f t="array" aca="1" ref="E11" ca="1">INDIRECT("'Raw Data'!"&amp;$H$5&amp;$B11+1)</f>
@@ -7243,7 +7241,7 @@
       <c r="G11" s="24"/>
       <c r="I11" s="43" t="str">
         <f>I5</f>
-        <v>DRB HCOM</v>
+        <v>AIR ASIA</v>
       </c>
       <c r="J11" s="44">
         <v>0</v>
@@ -7253,7 +7251,7 @@
       </c>
       <c r="L11" s="43" t="str">
         <f>"Minimum Holding of "&amp;I11</f>
-        <v>Minimum Holding of DRB HCOM</v>
+        <v>Minimum Holding of AIR ASIA</v>
       </c>
       <c r="M11" s="47">
         <v>0</v>
@@ -7274,7 +7272,7 @@
       <c r="AA11" s="22"/>
       <c r="AB11" s="22"/>
     </row>
-    <row r="12" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="29">
         <v>43709</v>
       </c>
@@ -7283,11 +7281,11 @@
       </c>
       <c r="C12" s="21" cm="1">
         <f t="array" aca="1" ref="C12" ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B12+1)</f>
-        <v>-5.9516154959009769E-2</v>
+        <v>8.5227272727272679E-2</v>
       </c>
       <c r="D12" s="21" cm="1">
         <f t="array" aca="1" ref="D12" ca="1">INDIRECT("'Raw Data'!"&amp;$H$4&amp;$B12+1)</f>
-        <v>8.5227272727272679E-2</v>
+        <v>-5.9516154959009769E-2</v>
       </c>
       <c r="E12" s="21" cm="1">
         <f t="array" aca="1" ref="E12" ca="1">INDIRECT("'Raw Data'!"&amp;$H$5&amp;$B12+1)</f>
@@ -7300,7 +7298,7 @@
       <c r="G12" s="24"/>
       <c r="I12" s="43" t="str">
         <f>I6</f>
-        <v>AIR ASIA</v>
+        <v>DRB HCOM</v>
       </c>
       <c r="J12" s="44">
         <v>0.10752586468155247</v>
@@ -7310,7 +7308,7 @@
       </c>
       <c r="L12" s="43" t="str">
         <f t="shared" ref="L12:L14" si="0">"Minimum Holding of "&amp;I12</f>
-        <v>Minimum Holding of AIR ASIA</v>
+        <v>Minimum Holding of DRB HCOM</v>
       </c>
       <c r="M12" s="47">
         <v>0</v>
@@ -7331,7 +7329,7 @@
       <c r="AA12" s="22"/>
       <c r="AB12" s="22"/>
     </row>
-    <row r="13" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="28">
         <v>43678</v>
       </c>
@@ -7340,11 +7338,11 @@
       </c>
       <c r="C13" s="21" cm="1">
         <f t="array" aca="1" ref="C13" ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B13+1)</f>
-        <v>-4.9031222532196994E-2</v>
+        <v>-1.6759776536312863E-2</v>
       </c>
       <c r="D13" s="21" cm="1">
         <f t="array" aca="1" ref="D13" ca="1">INDIRECT("'Raw Data'!"&amp;$H$4&amp;$B13+1)</f>
-        <v>-1.6759776536312863E-2</v>
+        <v>-4.9031222532196994E-2</v>
       </c>
       <c r="E13" s="21" cm="1">
         <f t="array" aca="1" ref="E13" ca="1">INDIRECT("'Raw Data'!"&amp;$H$5&amp;$B13+1)</f>
@@ -7388,7 +7386,7 @@
       <c r="AA13" s="22"/>
       <c r="AB13" s="22"/>
     </row>
-    <row r="14" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="29">
         <v>43647</v>
       </c>
@@ -7397,11 +7395,11 @@
       </c>
       <c r="C14" s="21" cm="1">
         <f t="array" aca="1" ref="C14" ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B14+1)</f>
-        <v>0.20452034616092785</v>
+        <v>1.3978566644340251</v>
       </c>
       <c r="D14" s="21" cm="1">
         <f t="array" aca="1" ref="D14" ca="1">INDIRECT("'Raw Data'!"&amp;$H$4&amp;$B14+1)</f>
-        <v>1.3978566644340251</v>
+        <v>0.20452034616092785</v>
       </c>
       <c r="E14" s="21" cm="1">
         <f t="array" aca="1" ref="E14" ca="1">INDIRECT("'Raw Data'!"&amp;$H$5&amp;$B14+1)</f>
@@ -7445,7 +7443,7 @@
       <c r="AA14" s="22"/>
       <c r="AB14" s="22"/>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A15" s="28">
         <v>43617</v>
       </c>
@@ -7454,11 +7452,11 @@
       </c>
       <c r="C15" s="21" cm="1">
         <f t="array" aca="1" ref="C15" ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B15+1)</f>
-        <v>5.7695116607429792E-2</v>
+        <v>-0.28207347566839774</v>
       </c>
       <c r="D15" s="21" cm="1">
         <f t="array" aca="1" ref="D15" ca="1">INDIRECT("'Raw Data'!"&amp;$H$4&amp;$B15+1)</f>
-        <v>-0.28207347566839774</v>
+        <v>5.7695116607429792E-2</v>
       </c>
       <c r="E15" s="21" cm="1">
         <f t="array" aca="1" ref="E15" ca="1">INDIRECT("'Raw Data'!"&amp;$H$5&amp;$B15+1)</f>
@@ -7494,7 +7492,7 @@
       <c r="AA15" s="22"/>
       <c r="AB15" s="22"/>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A16" s="29">
         <v>43586</v>
       </c>
@@ -7503,11 +7501,11 @@
       </c>
       <c r="C16" s="21" cm="1">
         <f t="array" aca="1" ref="C16" ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B16+1)</f>
-        <v>-4.5851528384279479E-2</v>
+        <v>-5.532842736440443E-2</v>
       </c>
       <c r="D16" s="21" cm="1">
         <f t="array" aca="1" ref="D16" ca="1">INDIRECT("'Raw Data'!"&amp;$H$4&amp;$B16+1)</f>
-        <v>-5.532842736440443E-2</v>
+        <v>-4.5851528384279479E-2</v>
       </c>
       <c r="E16" s="21" cm="1">
         <f t="array" aca="1" ref="E16" ca="1">INDIRECT("'Raw Data'!"&amp;$H$5&amp;$B16+1)</f>
@@ -7548,7 +7546,7 @@
       <c r="AA16" s="22"/>
       <c r="AB16" s="22"/>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A17" s="28">
         <v>43556</v>
       </c>
@@ -7557,11 +7555,11 @@
       </c>
       <c r="C17" s="21" cm="1">
         <f t="array" aca="1" ref="C17" ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B17+1)</f>
-        <v>0.14731904914188251</v>
+        <v>5.8568955568378489E-2</v>
       </c>
       <c r="D17" s="21" cm="1">
         <f t="array" aca="1" ref="D17" ca="1">INDIRECT("'Raw Data'!"&amp;$H$4&amp;$B17+1)</f>
-        <v>5.8568955568378489E-2</v>
+        <v>0.14731904914188251</v>
       </c>
       <c r="E17" s="21" cm="1">
         <f t="array" aca="1" ref="E17" ca="1">INDIRECT("'Raw Data'!"&amp;$H$5&amp;$B17+1)</f>
@@ -7593,7 +7591,7 @@
       <c r="AA17" s="22"/>
       <c r="AB17" s="22"/>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A18" s="29">
         <v>43525</v>
       </c>
@@ -7602,11 +7600,11 @@
       </c>
       <c r="C18" s="21" cm="1">
         <f t="array" aca="1" ref="C18" ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B18+1)</f>
-        <v>2.7041821764834745E-2</v>
+        <v>7.1185742247862421E-2</v>
       </c>
       <c r="D18" s="21" cm="1">
         <f t="array" aca="1" ref="D18" ca="1">INDIRECT("'Raw Data'!"&amp;$H$4&amp;$B18+1)</f>
-        <v>7.1185742247862421E-2</v>
+        <v>2.7041821764834745E-2</v>
       </c>
       <c r="E18" s="21" cm="1">
         <f t="array" aca="1" ref="E18" ca="1">INDIRECT("'Raw Data'!"&amp;$H$5&amp;$B18+1)</f>
@@ -7640,7 +7638,7 @@
       <c r="AA18" s="22"/>
       <c r="AB18" s="22"/>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A19" s="28">
         <v>43497</v>
       </c>
@@ -7649,11 +7647,11 @@
       </c>
       <c r="C19" s="21" cm="1">
         <f t="array" aca="1" ref="C19" ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B19+1)</f>
-        <v>0.14196411827217609</v>
+        <v>-3.9766544663171338E-2</v>
       </c>
       <c r="D19" s="21" cm="1">
         <f t="array" aca="1" ref="D19" ca="1">INDIRECT("'Raw Data'!"&amp;$H$4&amp;$B19+1)</f>
-        <v>-3.9766544663171338E-2</v>
+        <v>0.14196411827217609</v>
       </c>
       <c r="E19" s="21" cm="1">
         <f t="array" aca="1" ref="E19" ca="1">INDIRECT("'Raw Data'!"&amp;$H$5&amp;$B19+1)</f>
@@ -7691,7 +7689,7 @@
       <c r="AA19" s="22"/>
       <c r="AB19" s="22"/>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A20" s="29">
         <v>43466</v>
       </c>
@@ -7700,11 +7698,11 @@
       </c>
       <c r="C20" s="21" cm="1">
         <f t="array" aca="1" ref="C20" ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B20+1)</f>
-        <v>-4.7060225174242076E-2</v>
+        <v>-8.8786731566612612E-2</v>
       </c>
       <c r="D20" s="21" cm="1">
         <f t="array" aca="1" ref="D20" ca="1">INDIRECT("'Raw Data'!"&amp;$H$4&amp;$B20+1)</f>
-        <v>-8.8786731566612612E-2</v>
+        <v>-4.7060225174242076E-2</v>
       </c>
       <c r="E20" s="21" cm="1">
         <f t="array" aca="1" ref="E20" ca="1">INDIRECT("'Raw Data'!"&amp;$H$5&amp;$B20+1)</f>
@@ -7720,11 +7718,11 @@
       </c>
       <c r="J20" s="51" cm="1">
         <f t="array" aca="1" ref="J20" ca="1">MMULT(TRANSPOSE(J11:J14),MMULT(J30:M33,J11:J14))</f>
-        <v>1.0975495250415589E-2</v>
+        <v>1.1100794146351909E-2</v>
       </c>
       <c r="K20" s="37">
         <f ca="1">J20*12</f>
-        <v>0.13170594300498706</v>
+        <v>0.13320952975622291</v>
       </c>
       <c r="L20" s="51" t="s">
         <v>32</v>
@@ -7746,7 +7744,7 @@
       <c r="AA20" s="22"/>
       <c r="AB20" s="22"/>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A21" s="28">
         <v>43435</v>
       </c>
@@ -7755,11 +7753,11 @@
       </c>
       <c r="C21" s="21" cm="1">
         <f t="array" aca="1" ref="C21" ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B21+1)</f>
-        <v>-8.1070724764615673E-2</v>
+        <v>0.17858281100605536</v>
       </c>
       <c r="D21" s="21" cm="1">
         <f t="array" aca="1" ref="D21" ca="1">INDIRECT("'Raw Data'!"&amp;$H$4&amp;$B21+1)</f>
-        <v>0.17858281100605536</v>
+        <v>-8.1070724764615673E-2</v>
       </c>
       <c r="E21" s="21" cm="1">
         <f t="array" aca="1" ref="E21" ca="1">INDIRECT("'Raw Data'!"&amp;$H$5&amp;$B21+1)</f>
@@ -7775,11 +7773,11 @@
       </c>
       <c r="J21" s="52">
         <f ca="1">SQRT(SUM(J20))</f>
-        <v>0.10476399787338964</v>
+        <v>0.105360306312918</v>
       </c>
       <c r="K21" s="35">
         <f ca="1">J21*SQRT(12)</f>
-        <v>0.36291313424149729</v>
+        <v>0.36497880726998777</v>
       </c>
       <c r="L21" s="51" t="str">
         <f ca="1">IF(K21&lt;0.15,"Low Risk","High Risk")</f>
@@ -7802,7 +7800,7 @@
       <c r="AA21" s="22"/>
       <c r="AB21" s="22"/>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A22" s="29">
         <v>43405</v>
       </c>
@@ -7811,11 +7809,11 @@
       </c>
       <c r="C22" s="21" cm="1">
         <f t="array" aca="1" ref="C22" ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B22+1)</f>
-        <v>-1.5944839474251276E-2</v>
+        <v>-3.5652084827374184E-2</v>
       </c>
       <c r="D22" s="21" cm="1">
         <f t="array" aca="1" ref="D22" ca="1">INDIRECT("'Raw Data'!"&amp;$H$4&amp;$B22+1)</f>
-        <v>-3.5652084827374184E-2</v>
+        <v>-1.5944839474251276E-2</v>
       </c>
       <c r="E22" s="21" cm="1">
         <f t="array" aca="1" ref="E22" ca="1">INDIRECT("'Raw Data'!"&amp;$H$5&amp;$B22+1)</f>
@@ -7831,11 +7829,11 @@
       </c>
       <c r="J22" s="52">
         <f ca="1">SUMPRODUCT(J5:J8,J11:J14)</f>
-        <v>4.1716259802769849E-2</v>
+        <v>4.0023746281319487E-2</v>
       </c>
       <c r="K22" s="35">
         <f ca="1">((1+J22)^12)-1</f>
-        <v>0.6330268133993957</v>
+        <v>0.60147094937053458</v>
       </c>
       <c r="L22" s="51" t="str">
         <f ca="1">IF(K22&lt;0.15,"Low Return","High Return")</f>
@@ -7858,7 +7856,7 @@
       <c r="AA22" s="22"/>
       <c r="AB22" s="22"/>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A23" s="28">
         <v>43374</v>
       </c>
@@ -7867,11 +7865,11 @@
       </c>
       <c r="C23" s="21" cm="1">
         <f t="array" aca="1" ref="C23" ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B23+1)</f>
-        <v>-0.12110595587539059</v>
+        <v>0.17108578284343126</v>
       </c>
       <c r="D23" s="21" cm="1">
         <f t="array" aca="1" ref="D23" ca="1">INDIRECT("'Raw Data'!"&amp;$H$4&amp;$B23+1)</f>
-        <v>0.17108578284343126</v>
+        <v>-0.12110595587539059</v>
       </c>
       <c r="E23" s="21" cm="1">
         <f t="array" aca="1" ref="E23" ca="1">INDIRECT("'Raw Data'!"&amp;$H$5&amp;$B23+1)</f>
@@ -7890,7 +7888,7 @@
       </c>
       <c r="K23" s="49">
         <f ca="1">(K22-J27)/K21</f>
-        <v>1.6726504392520969</v>
+        <v>1.5767242861990018</v>
       </c>
       <c r="L23" s="51" t="str">
         <f ca="1">IF(K23&lt;1,"Not an ideal portfolio","Ideal Portfolio")</f>
@@ -7913,7 +7911,7 @@
       <c r="AA23" s="22"/>
       <c r="AB23" s="22"/>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A24" s="29">
         <v>43344</v>
       </c>
@@ -7922,11 +7920,11 @@
       </c>
       <c r="C24" s="21" cm="1">
         <f t="array" aca="1" ref="C24" ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B24+1)</f>
-        <v>-4.403711246888424E-2</v>
+        <v>-0.16774837743384927</v>
       </c>
       <c r="D24" s="21" cm="1">
         <f t="array" aca="1" ref="D24" ca="1">INDIRECT("'Raw Data'!"&amp;$H$4&amp;$B24+1)</f>
-        <v>-0.16774837743384927</v>
+        <v>-4.403711246888424E-2</v>
       </c>
       <c r="E24" s="21" cm="1">
         <f t="array" aca="1" ref="E24" ca="1">INDIRECT("'Raw Data'!"&amp;$H$5&amp;$B24+1)</f>
@@ -7955,7 +7953,7 @@
       <c r="AA24" s="22"/>
       <c r="AB24" s="22"/>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A25" s="28">
         <v>43313</v>
       </c>
@@ -7964,11 +7962,11 @@
       </c>
       <c r="C25" s="21" cm="1">
         <f t="array" aca="1" ref="C25" ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B25+1)</f>
-        <v>2.2537948907811804E-2</v>
+        <v>-8.1361218125114654E-2</v>
       </c>
       <c r="D25" s="21" cm="1">
         <f t="array" aca="1" ref="D25" ca="1">INDIRECT("'Raw Data'!"&amp;$H$4&amp;$B25+1)</f>
-        <v>-8.1361218125114654E-2</v>
+        <v>2.2537948907811804E-2</v>
       </c>
       <c r="E25" s="21" cm="1">
         <f t="array" aca="1" ref="E25" ca="1">INDIRECT("'Raw Data'!"&amp;$H$5&amp;$B25+1)</f>
@@ -8002,7 +8000,7 @@
       <c r="AA25" s="22"/>
       <c r="AB25" s="22"/>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A26" s="29">
         <v>43282</v>
       </c>
@@ -8011,11 +8009,11 @@
       </c>
       <c r="C26" s="21" cm="1">
         <f t="array" aca="1" ref="C26" ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B26+1)</f>
-        <v>0.13267285212559632</v>
+        <v>-3.3681971281687671E-2</v>
       </c>
       <c r="D26" s="21" cm="1">
         <f t="array" aca="1" ref="D26" ca="1">INDIRECT("'Raw Data'!"&amp;$H$4&amp;$B26+1)</f>
-        <v>-3.3681971281687671E-2</v>
+        <v>0.13267285212559632</v>
       </c>
       <c r="E26" s="21" cm="1">
         <f t="array" aca="1" ref="E26" ca="1">INDIRECT("'Raw Data'!"&amp;$H$5&amp;$B26+1)</f>
@@ -8051,7 +8049,7 @@
       <c r="AA26" s="22"/>
       <c r="AB26" s="22"/>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A27" s="28">
         <v>43252</v>
       </c>
@@ -8060,11 +8058,11 @@
       </c>
       <c r="C27" s="21" cm="1">
         <f t="array" aca="1" ref="C27" ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B27+1)</f>
-        <v>0.12641709966934339</v>
+        <v>0.23597721297107818</v>
       </c>
       <c r="D27" s="21" cm="1">
         <f t="array" aca="1" ref="D27" ca="1">INDIRECT("'Raw Data'!"&amp;$H$4&amp;$B27+1)</f>
-        <v>0.23597721297107818</v>
+        <v>0.12641709966934339</v>
       </c>
       <c r="E27" s="21" cm="1">
         <f t="array" aca="1" ref="E27" ca="1">INDIRECT("'Raw Data'!"&amp;$H$5&amp;$B27+1)</f>
@@ -8100,7 +8098,7 @@
       <c r="AA27" s="22"/>
       <c r="AB27" s="22"/>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A28" s="29">
         <v>43221</v>
       </c>
@@ -8109,11 +8107,11 @@
       </c>
       <c r="C28" s="21" cm="1">
         <f t="array" aca="1" ref="C28" ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B28+1)</f>
-        <v>-0.19818199034182371</v>
+        <v>-2.9245985323832904E-2</v>
       </c>
       <c r="D28" s="21" cm="1">
         <f t="array" aca="1" ref="D28" ca="1">INDIRECT("'Raw Data'!"&amp;$H$4&amp;$B28+1)</f>
-        <v>-2.9245985323832904E-2</v>
+        <v>-0.19818199034182371</v>
       </c>
       <c r="E28" s="21" cm="1">
         <f t="array" aca="1" ref="E28" ca="1">INDIRECT("'Raw Data'!"&amp;$H$5&amp;$B28+1)</f>
@@ -8145,7 +8143,7 @@
       <c r="AA28" s="22"/>
       <c r="AB28" s="22"/>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A29" s="28">
         <v>43191</v>
       </c>
@@ -8154,11 +8152,11 @@
       </c>
       <c r="C29" s="21" cm="1">
         <f t="array" aca="1" ref="C29" ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B29+1)</f>
-        <v>-0.11065263157894734</v>
+        <v>-0.20001701548409051</v>
       </c>
       <c r="D29" s="21" cm="1">
         <f t="array" aca="1" ref="D29" ca="1">INDIRECT("'Raw Data'!"&amp;$H$4&amp;$B29+1)</f>
-        <v>-0.20001701548409051</v>
+        <v>-0.11065263157894734</v>
       </c>
       <c r="E29" s="21" cm="1">
         <f t="array" aca="1" ref="E29" ca="1">INDIRECT("'Raw Data'!"&amp;$H$5&amp;$B29+1)</f>
@@ -8174,11 +8172,11 @@
       </c>
       <c r="J29" s="14" t="str">
         <f>I5</f>
-        <v>DRB HCOM</v>
+        <v>AIR ASIA</v>
       </c>
       <c r="K29" s="14" t="str">
         <f>I6</f>
-        <v>AIR ASIA</v>
+        <v>DRB HCOM</v>
       </c>
       <c r="L29" s="14" t="str">
         <f>I7</f>
@@ -8204,7 +8202,7 @@
       <c r="AA29" s="22"/>
       <c r="AB29" s="22"/>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A30" s="29">
         <v>43160</v>
       </c>
@@ -8213,11 +8211,11 @@
       </c>
       <c r="C30" s="21" cm="1">
         <f t="array" aca="1" ref="C30" ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B30+1)</f>
-        <v>-6.8700494078895696E-2</v>
+        <v>-2.0336722787131171E-2</v>
       </c>
       <c r="D30" s="21" cm="1">
         <f t="array" aca="1" ref="D30" ca="1">INDIRECT("'Raw Data'!"&amp;$H$4&amp;$B30+1)</f>
-        <v>-2.0336722787131171E-2</v>
+        <v>-6.8700494078895696E-2</v>
       </c>
       <c r="E30" s="21" cm="1">
         <f t="array" aca="1" ref="E30" ca="1">INDIRECT("'Raw Data'!"&amp;$H$5&amp;$B30+1)</f>
@@ -8233,7 +8231,7 @@
       </c>
       <c r="J30" s="37" cm="1">
         <f t="array" aca="1" ref="J30" ca="1">+_xlfn.VAR.S(IF(ISERROR(C3:C73),"",C3:C73))</f>
-        <v>1.6636691360429175E-2</v>
+        <v>4.918886945513512E-2</v>
       </c>
       <c r="K30" s="37" cm="1">
         <f t="array" aca="1" ref="K30" ca="1">_xlfn.COVARIANCE.S(IF(ISERROR(C3:C73),"",C3:C73),IF(ISERROR(D3:D73),"",D3:D73))</f>
@@ -8241,11 +8239,11 @@
       </c>
       <c r="L30" s="37" cm="1">
         <f t="array" aca="1" ref="L30" ca="1">_xlfn.COVARIANCE.S(IF(ISERROR(C3:C73),"",C3:C73),IF(ISERROR(E3:E73),"",E3:E73))</f>
-        <v>7.8394024209790664E-3</v>
+        <v>6.7668022502725554E-4</v>
       </c>
       <c r="M30" s="37" cm="1">
         <f t="array" aca="1" ref="M30" ca="1">_xlfn.COVARIANCE.S(IF(ISERROR(C3:C73),"",C3:C73),IF(ISERROR(F3:F73),"",F3:F73))</f>
-        <v>2.2834644320297061E-3</v>
+        <v>1.0819340788869106E-3</v>
       </c>
       <c r="N30" s="22"/>
       <c r="O30" s="22"/>
@@ -8263,7 +8261,7 @@
       <c r="AA30" s="22"/>
       <c r="AB30" s="22"/>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A31" s="28">
         <v>43132</v>
       </c>
@@ -8272,11 +8270,11 @@
       </c>
       <c r="C31" s="21" cm="1">
         <f t="array" aca="1" ref="C31" ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B31+1)</f>
-        <v>7.7053779586675033E-3</v>
+        <v>-0.10275201914448098</v>
       </c>
       <c r="D31" s="21" cm="1">
         <f t="array" aca="1" ref="D31" ca="1">INDIRECT("'Raw Data'!"&amp;$H$4&amp;$B31+1)</f>
-        <v>-0.10275201914448098</v>
+        <v>7.7053779586675033E-3</v>
       </c>
       <c r="E31" s="21" cm="1">
         <f t="array" aca="1" ref="E31" ca="1">INDIRECT("'Raw Data'!"&amp;$H$5&amp;$B31+1)</f>
@@ -8296,15 +8294,15 @@
       </c>
       <c r="K31" s="37" cm="1">
         <f t="array" aca="1" ref="K31" ca="1">+_xlfn.VAR.S(IF(ISERROR(D3:D73),"",(D3:D73)))</f>
-        <v>4.918886945513512E-2</v>
+        <v>1.6636691360429175E-2</v>
       </c>
       <c r="L31" s="37" cm="1">
         <f t="array" aca="1" ref="L31" ca="1">_xlfn.COVARIANCE.S(IF(ISERROR(D3:D73),"",D3:D73),IF(ISERROR(E3:E73),"",E3:E73))</f>
-        <v>6.7668022502725554E-4</v>
+        <v>7.8394024209790664E-3</v>
       </c>
       <c r="M31" s="37" cm="1">
         <f t="array" aca="1" ref="M31" ca="1">_xlfn.COVARIANCE.S(IF(ISERROR(D3:D73),"",D3:D73),IF(ISERROR(F3:F73),"",F3:F73))</f>
-        <v>1.0819340788869106E-3</v>
+        <v>2.2834644320297061E-3</v>
       </c>
       <c r="N31" s="22"/>
       <c r="O31" s="22"/>
@@ -8322,7 +8320,7 @@
       <c r="AA31" s="22"/>
       <c r="AB31" s="22"/>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A32" s="29">
         <v>43101</v>
       </c>
@@ -8331,11 +8329,11 @@
       </c>
       <c r="C32" s="21" cm="1">
         <f t="array" aca="1" ref="C32" ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B32+1)</f>
-        <v>0.42078374129800139</v>
+        <v>5.7995094548619286E-2</v>
       </c>
       <c r="D32" s="21" cm="1">
         <f t="array" aca="1" ref="D32" ca="1">INDIRECT("'Raw Data'!"&amp;$H$4&amp;$B32+1)</f>
-        <v>5.7995094548619286E-2</v>
+        <v>0.42078374129800139</v>
       </c>
       <c r="E32" s="21" cm="1">
         <f t="array" aca="1" ref="E32" ca="1">INDIRECT("'Raw Data'!"&amp;$H$5&amp;$B32+1)</f>
@@ -8351,11 +8349,11 @@
       </c>
       <c r="J32" s="37">
         <f ca="1">L30</f>
-        <v>7.8394024209790664E-3</v>
+        <v>6.7668022502725554E-4</v>
       </c>
       <c r="K32" s="37">
         <f ca="1">L31</f>
-        <v>6.7668022502725554E-4</v>
+        <v>7.8394024209790664E-3</v>
       </c>
       <c r="L32" s="37" cm="1">
         <f t="array" aca="1" ref="L32" ca="1">+_xlfn.VAR.S(IF(ISERROR(E3:E73),"",(E3:E73)))</f>
@@ -8381,7 +8379,7 @@
       <c r="AA32" s="22"/>
       <c r="AB32" s="22"/>
     </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A33" s="28">
         <v>43070</v>
       </c>
@@ -8390,11 +8388,11 @@
       </c>
       <c r="C33" s="21" cm="1">
         <f t="array" aca="1" ref="C33" ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B33+1)</f>
-        <v>7.0175438596491099E-2</v>
+        <v>0.23584628923437967</v>
       </c>
       <c r="D33" s="21" cm="1">
         <f t="array" aca="1" ref="D33" ca="1">INDIRECT("'Raw Data'!"&amp;$H$4&amp;$B33+1)</f>
-        <v>0.23584628923437967</v>
+        <v>7.0175438596491099E-2</v>
       </c>
       <c r="E33" s="21" cm="1">
         <f t="array" aca="1" ref="E33" ca="1">INDIRECT("'Raw Data'!"&amp;$H$5&amp;$B33+1)</f>
@@ -8410,11 +8408,11 @@
       </c>
       <c r="J33" s="37">
         <f ca="1">M30</f>
-        <v>2.2834644320297061E-3</v>
+        <v>1.0819340788869106E-3</v>
       </c>
       <c r="K33" s="37">
         <f ca="1">M31</f>
-        <v>1.0819340788869106E-3</v>
+        <v>2.2834644320297061E-3</v>
       </c>
       <c r="L33" s="37">
         <f ca="1">M32</f>
@@ -8440,7 +8438,7 @@
       <c r="AA33" s="22"/>
       <c r="AB33" s="22"/>
     </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A34" s="29">
         <v>43040</v>
       </c>
@@ -8449,11 +8447,11 @@
       </c>
       <c r="C34" s="21" cm="1">
         <f t="array" aca="1" ref="C34" ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B34+1)</f>
-        <v>5.8620898047984779E-3</v>
+        <v>6.6868349676611663E-2</v>
       </c>
       <c r="D34" s="21" cm="1">
         <f t="array" aca="1" ref="D34" ca="1">INDIRECT("'Raw Data'!"&amp;$H$4&amp;$B34+1)</f>
-        <v>6.6868349676611663E-2</v>
+        <v>5.8620898047984779E-3</v>
       </c>
       <c r="E34" s="21" cm="1">
         <f t="array" aca="1" ref="E34" ca="1">INDIRECT("'Raw Data'!"&amp;$H$5&amp;$B34+1)</f>
@@ -8485,7 +8483,7 @@
       <c r="AA34" s="22"/>
       <c r="AB34" s="22"/>
     </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A35" s="28">
         <v>43009</v>
       </c>
@@ -8494,11 +8492,11 @@
       </c>
       <c r="C35" s="21" cm="1">
         <f t="array" aca="1" ref="C35" ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B35+1)</f>
-        <v>4.947041288767684E-2</v>
+        <v>-5.9919584191428892E-2</v>
       </c>
       <c r="D35" s="21" cm="1">
         <f t="array" aca="1" ref="D35" ca="1">INDIRECT("'Raw Data'!"&amp;$H$4&amp;$B35+1)</f>
-        <v>-5.9919584191428892E-2</v>
+        <v>4.947041288767684E-2</v>
       </c>
       <c r="E35" s="21" cm="1">
         <f t="array" aca="1" ref="E35" ca="1">INDIRECT("'Raw Data'!"&amp;$H$5&amp;$B35+1)</f>
@@ -8532,7 +8530,7 @@
       <c r="AA35" s="22"/>
       <c r="AB35" s="22"/>
     </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A36" s="29">
         <v>42979</v>
       </c>
@@ -8541,11 +8539,11 @@
       </c>
       <c r="C36" s="21" cm="1">
         <f t="array" aca="1" ref="C36" ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B36+1)</f>
-        <v>3.1669174900215924E-2</v>
+        <v>2.9507229271172556E-3</v>
       </c>
       <c r="D36" s="21" cm="1">
         <f t="array" aca="1" ref="D36" ca="1">INDIRECT("'Raw Data'!"&amp;$H$4&amp;$B36+1)</f>
-        <v>2.9507229271172556E-3</v>
+        <v>3.1669174900215924E-2</v>
       </c>
       <c r="E36" s="21" cm="1">
         <f t="array" aca="1" ref="E36" ca="1">INDIRECT("'Raw Data'!"&amp;$H$5&amp;$B36+1)</f>
@@ -8579,7 +8577,7 @@
       <c r="AA36" s="22"/>
       <c r="AB36" s="22"/>
     </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A37" s="28">
         <v>42948</v>
       </c>
@@ -8588,11 +8586,11 @@
       </c>
       <c r="C37" s="21" cm="1">
         <f t="array" aca="1" ref="C37" ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B37+1)</f>
-        <v>-6.5088395424236889E-2</v>
+        <v>3.9145543744889502E-2</v>
       </c>
       <c r="D37" s="21" cm="1">
         <f t="array" aca="1" ref="D37" ca="1">INDIRECT("'Raw Data'!"&amp;$H$4&amp;$B37+1)</f>
-        <v>3.9145543744889502E-2</v>
+        <v>-6.5088395424236889E-2</v>
       </c>
       <c r="E37" s="21" cm="1">
         <f t="array" aca="1" ref="E37" ca="1">INDIRECT("'Raw Data'!"&amp;$H$5&amp;$B37+1)</f>
@@ -8626,7 +8624,7 @@
       <c r="AA37" s="22"/>
       <c r="AB37" s="22"/>
     </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A38" s="29">
         <v>42917</v>
       </c>
@@ -8635,11 +8633,11 @@
       </c>
       <c r="C38" s="21" cm="1">
         <f t="array" aca="1" ref="C38" ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B38+1)</f>
-        <v>-5.0586595423394096E-2</v>
+        <v>2.7839058724656036E-2</v>
       </c>
       <c r="D38" s="21" cm="1">
         <f t="array" aca="1" ref="D38" ca="1">INDIRECT("'Raw Data'!"&amp;$H$4&amp;$B38+1)</f>
-        <v>2.7839058724656036E-2</v>
+        <v>-5.0586595423394096E-2</v>
       </c>
       <c r="E38" s="21" cm="1">
         <f t="array" aca="1" ref="E38" ca="1">INDIRECT("'Raw Data'!"&amp;$H$5&amp;$B38+1)</f>
@@ -8673,7 +8671,7 @@
       <c r="AA38" s="22"/>
       <c r="AB38" s="22"/>
     </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A39" s="28">
         <v>42887</v>
       </c>
@@ -8682,11 +8680,11 @@
       </c>
       <c r="C39" s="21" cm="1">
         <f t="array" aca="1" ref="C39" ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B39+1)</f>
-        <v>0.13373279778758151</v>
+        <v>-6.1599498851534935E-3</v>
       </c>
       <c r="D39" s="21" cm="1">
         <f t="array" aca="1" ref="D39" ca="1">INDIRECT("'Raw Data'!"&amp;$H$4&amp;$B39+1)</f>
-        <v>-6.1599498851534935E-3</v>
+        <v>0.13373279778758151</v>
       </c>
       <c r="E39" s="21" cm="1">
         <f t="array" aca="1" ref="E39" ca="1">INDIRECT("'Raw Data'!"&amp;$H$5&amp;$B39+1)</f>
@@ -8720,7 +8718,7 @@
       <c r="AA39" s="22"/>
       <c r="AB39" s="22"/>
     </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A40" s="29">
         <v>42856</v>
       </c>
@@ -8729,11 +8727,11 @@
       </c>
       <c r="C40" s="21" cm="1">
         <f t="array" aca="1" ref="C40" ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B40+1)</f>
-        <v>9.0315169789647431E-2</v>
+        <v>0.12908169279735934</v>
       </c>
       <c r="D40" s="21" cm="1">
         <f t="array" aca="1" ref="D40" ca="1">INDIRECT("'Raw Data'!"&amp;$H$4&amp;$B40+1)</f>
-        <v>0.12908169279735934</v>
+        <v>9.0315169789647431E-2</v>
       </c>
       <c r="E40" s="21" cm="1">
         <f t="array" aca="1" ref="E40" ca="1">INDIRECT("'Raw Data'!"&amp;$H$5&amp;$B40+1)</f>
@@ -8767,7 +8765,7 @@
       <c r="AA40" s="22"/>
       <c r="AB40" s="22"/>
     </row>
-    <row r="41" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A41" s="28">
         <v>42826</v>
       </c>
@@ -8776,11 +8774,11 @@
       </c>
       <c r="C41" s="21" cm="1">
         <f t="array" aca="1" ref="C41" ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B41+1)</f>
-        <v>2.8577758085954773E-2</v>
+        <v>-0.11042365771812075</v>
       </c>
       <c r="D41" s="21" cm="1">
         <f t="array" aca="1" ref="D41" ca="1">INDIRECT("'Raw Data'!"&amp;$H$4&amp;$B41+1)</f>
-        <v>-0.11042365771812075</v>
+        <v>2.8577758085954773E-2</v>
       </c>
       <c r="E41" s="21" cm="1">
         <f t="array" aca="1" ref="E41" ca="1">INDIRECT("'Raw Data'!"&amp;$H$5&amp;$B41+1)</f>
@@ -8812,7 +8810,7 @@
       <c r="AA41" s="22"/>
       <c r="AB41" s="22"/>
     </row>
-    <row r="42" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A42" s="29">
         <v>42795</v>
       </c>
@@ -8821,11 +8819,11 @@
       </c>
       <c r="C42" s="21" cm="1">
         <f t="array" aca="1" ref="C42" ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B42+1)</f>
-        <v>-1.4123471170646376E-2</v>
+        <v>0.37287647566945004</v>
       </c>
       <c r="D42" s="21" cm="1">
         <f t="array" aca="1" ref="D42" ca="1">INDIRECT("'Raw Data'!"&amp;$H$4&amp;$B42+1)</f>
-        <v>0.37287647566945004</v>
+        <v>-1.4123471170646376E-2</v>
       </c>
       <c r="E42" s="21" cm="1">
         <f t="array" aca="1" ref="E42" ca="1">INDIRECT("'Raw Data'!"&amp;$H$5&amp;$B42+1)</f>
@@ -8859,7 +8857,7 @@
       <c r="AA42" s="22"/>
       <c r="AB42" s="22"/>
     </row>
-    <row r="43" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A43" s="28">
         <v>42767</v>
       </c>
@@ -8868,11 +8866,11 @@
       </c>
       <c r="C43" s="21" cm="1">
         <f t="array" aca="1" ref="C43" ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B43+1)</f>
-        <v>0.21374922682689759</v>
+        <v>6.5500843687682095E-2</v>
       </c>
       <c r="D43" s="21" cm="1">
         <f t="array" aca="1" ref="D43" ca="1">INDIRECT("'Raw Data'!"&amp;$H$4&amp;$B43+1)</f>
-        <v>6.5500843687682095E-2</v>
+        <v>0.21374922682689759</v>
       </c>
       <c r="E43" s="21" cm="1">
         <f t="array" aca="1" ref="E43" ca="1">INDIRECT("'Raw Data'!"&amp;$H$5&amp;$B43+1)</f>
@@ -8904,7 +8902,7 @@
       <c r="AA43" s="22"/>
       <c r="AB43" s="22"/>
     </row>
-    <row r="44" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A44" s="29">
         <v>42736</v>
       </c>
@@ -8913,11 +8911,11 @@
       </c>
       <c r="C44" s="21" cm="1">
         <f t="array" aca="1" ref="C44" ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B44+1)</f>
-        <v>1.7349874145990537E-2</v>
+        <v>-0.17029400534555164</v>
       </c>
       <c r="D44" s="21" cm="1">
         <f t="array" aca="1" ref="D44" ca="1">INDIRECT("'Raw Data'!"&amp;$H$4&amp;$B44+1)</f>
-        <v>-0.17029400534555164</v>
+        <v>1.7349874145990537E-2</v>
       </c>
       <c r="E44" s="21" cm="1">
         <f t="array" aca="1" ref="E44" ca="1">INDIRECT("'Raw Data'!"&amp;$H$5&amp;$B44+1)</f>
@@ -8949,7 +8947,7 @@
       <c r="AA44" s="22"/>
       <c r="AB44" s="22"/>
     </row>
-    <row r="45" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A45" s="28">
         <v>42705</v>
       </c>
@@ -8958,11 +8956,11 @@
       </c>
       <c r="C45" s="21" cm="1">
         <f t="array" aca="1" ref="C45" ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B45+1)</f>
-        <v>0.19177201628455115</v>
+        <v>-3.5510462904248885E-3</v>
       </c>
       <c r="D45" s="21" cm="1">
         <f t="array" aca="1" ref="D45" ca="1">INDIRECT("'Raw Data'!"&amp;$H$4&amp;$B45+1)</f>
-        <v>-3.5510462904248885E-3</v>
+        <v>0.19177201628455115</v>
       </c>
       <c r="E45" s="21" cm="1">
         <f t="array" aca="1" ref="E45" ca="1">INDIRECT("'Raw Data'!"&amp;$H$5&amp;$B45+1)</f>
@@ -8994,7 +8992,7 @@
       <c r="AA45" s="22"/>
       <c r="AB45" s="22"/>
     </row>
-    <row r="46" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A46" s="29">
         <v>42675</v>
       </c>
@@ -9003,11 +9001,11 @@
       </c>
       <c r="C46" s="21" cm="1">
         <f t="array" aca="1" ref="C46" ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B46+1)</f>
-        <v>-0.22923203963666397</v>
+        <v>-7.1770334928230144E-3</v>
       </c>
       <c r="D46" s="21" cm="1">
         <f t="array" aca="1" ref="D46" ca="1">INDIRECT("'Raw Data'!"&amp;$H$4&amp;$B46+1)</f>
-        <v>-7.1770334928230144E-3</v>
+        <v>-0.22923203963666397</v>
       </c>
       <c r="E46" s="21" cm="1">
         <f t="array" aca="1" ref="E46" ca="1">INDIRECT("'Raw Data'!"&amp;$H$5&amp;$B46+1)</f>
@@ -9039,7 +9037,7 @@
       <c r="AA46" s="22"/>
       <c r="AB46" s="22"/>
     </row>
-    <row r="47" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A47" s="28">
         <v>42644</v>
       </c>
@@ -9048,11 +9046,11 @@
       </c>
       <c r="C47" s="21" cm="1">
         <f t="array" aca="1" ref="C47" ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B47+1)</f>
-        <v>-0.12417733420120051</v>
+        <v>-5.1021627434579948E-2</v>
       </c>
       <c r="D47" s="21" cm="1">
         <f t="array" aca="1" ref="D47" ca="1">INDIRECT("'Raw Data'!"&amp;$H$4&amp;$B47+1)</f>
-        <v>-5.1021627434579948E-2</v>
+        <v>-0.12417733420120051</v>
       </c>
       <c r="E47" s="21" cm="1">
         <f t="array" aca="1" ref="E47" ca="1">INDIRECT("'Raw Data'!"&amp;$H$5&amp;$B47+1)</f>
@@ -9084,7 +9082,7 @@
       <c r="AA47" s="22"/>
       <c r="AB47" s="22"/>
     </row>
-    <row r="48" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A48" s="29">
         <v>42614</v>
       </c>
@@ -9093,11 +9091,11 @@
       </c>
       <c r="C48" s="21" cm="1">
         <f t="array" aca="1" ref="C48" ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B48+1)</f>
-        <v>0.10686839577329486</v>
+        <v>3.477218225419681E-3</v>
       </c>
       <c r="D48" s="21" cm="1">
         <f t="array" aca="1" ref="D48" ca="1">INDIRECT("'Raw Data'!"&amp;$H$4&amp;$B48+1)</f>
-        <v>3.477218225419681E-3</v>
+        <v>0.10686839577329486</v>
       </c>
       <c r="E48" s="21" cm="1">
         <f t="array" aca="1" ref="E48" ca="1">INDIRECT("'Raw Data'!"&amp;$H$5&amp;$B48+1)</f>
@@ -9129,7 +9127,7 @@
       <c r="AA48" s="22"/>
       <c r="AB48" s="22"/>
     </row>
-    <row r="49" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A49" s="28">
         <v>42583</v>
       </c>
@@ -9138,11 +9136,11 @@
       </c>
       <c r="C49" s="21" cm="1">
         <f t="array" aca="1" ref="C49" ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B49+1)</f>
-        <v>0.44750869061413684</v>
+        <v>0.1268747466558573</v>
       </c>
       <c r="D49" s="21" cm="1">
         <f t="array" aca="1" ref="D49" ca="1">INDIRECT("'Raw Data'!"&amp;$H$4&amp;$B49+1)</f>
-        <v>0.1268747466558573</v>
+        <v>0.44750869061413684</v>
       </c>
       <c r="E49" s="21" cm="1">
         <f t="array" aca="1" ref="E49" ca="1">INDIRECT("'Raw Data'!"&amp;$H$5&amp;$B49+1)</f>
@@ -9174,7 +9172,7 @@
       <c r="AA49" s="22"/>
       <c r="AB49" s="22"/>
     </row>
-    <row r="50" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A50" s="29">
         <v>42552</v>
       </c>
@@ -9183,11 +9181,11 @@
       </c>
       <c r="C50" s="21" cm="1">
         <f t="array" aca="1" ref="C50" ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B50+1)</f>
-        <v>-5.5312283936391178E-3</v>
+        <v>0.15083190794588708</v>
       </c>
       <c r="D50" s="21" cm="1">
         <f t="array" aca="1" ref="D50" ca="1">INDIRECT("'Raw Data'!"&amp;$H$4&amp;$B50+1)</f>
-        <v>0.15083190794588708</v>
+        <v>-5.5312283936391178E-3</v>
       </c>
       <c r="E50" s="21" cm="1">
         <f t="array" aca="1" ref="E50" ca="1">INDIRECT("'Raw Data'!"&amp;$H$5&amp;$B50+1)</f>
@@ -9219,7 +9217,7 @@
       <c r="AA50" s="22"/>
       <c r="AB50" s="22"/>
     </row>
-    <row r="51" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A51" s="28">
         <v>42522</v>
       </c>
@@ -9228,11 +9226,11 @@
       </c>
       <c r="C51" s="21" cm="1">
         <f t="array" aca="1" ref="C51" ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B51+1)</f>
-        <v>0.13750163848472932</v>
+        <v>0.21042725390551481</v>
       </c>
       <c r="D51" s="21" cm="1">
         <f t="array" aca="1" ref="D51" ca="1">INDIRECT("'Raw Data'!"&amp;$H$4&amp;$B51+1)</f>
-        <v>0.21042725390551481</v>
+        <v>0.13750163848472932</v>
       </c>
       <c r="E51" s="21" cm="1">
         <f t="array" aca="1" ref="E51" ca="1">INDIRECT("'Raw Data'!"&amp;$H$5&amp;$B51+1)</f>
@@ -9264,7 +9262,7 @@
       <c r="AA51" s="22"/>
       <c r="AB51" s="22"/>
     </row>
-    <row r="52" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A52" s="29">
         <v>42491</v>
       </c>
@@ -9273,11 +9271,11 @@
       </c>
       <c r="C52" s="21" cm="1">
         <f t="array" aca="1" ref="C52" ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B52+1)</f>
-        <v>-0.17524324324324325</v>
+        <v>3.8303693570451339E-2</v>
       </c>
       <c r="D52" s="21" cm="1">
         <f t="array" aca="1" ref="D52" ca="1">INDIRECT("'Raw Data'!"&amp;$H$4&amp;$B52+1)</f>
-        <v>3.8303693570451339E-2</v>
+        <v>-0.17524324324324325</v>
       </c>
       <c r="E52" s="21" cm="1">
         <f t="array" aca="1" ref="E52" ca="1">INDIRECT("'Raw Data'!"&amp;$H$5&amp;$B52+1)</f>
@@ -9309,7 +9307,7 @@
       <c r="AA52" s="22"/>
       <c r="AB52" s="22"/>
     </row>
-    <row r="53" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A53" s="28">
         <v>42461</v>
       </c>
@@ -9318,11 +9316,11 @@
       </c>
       <c r="C53" s="21" cm="1">
         <f t="array" aca="1" ref="C53" ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B53+1)</f>
-        <v>-4.8940982932346264E-2</v>
+        <v>0.24501216545012183</v>
       </c>
       <c r="D53" s="21" cm="1">
         <f t="array" aca="1" ref="D53" ca="1">INDIRECT("'Raw Data'!"&amp;$H$4&amp;$B53+1)</f>
-        <v>0.24501216545012183</v>
+        <v>-4.8940982932346264E-2</v>
       </c>
       <c r="E53" s="21" cm="1">
         <f t="array" aca="1" ref="E53" ca="1">INDIRECT("'Raw Data'!"&amp;$H$5&amp;$B53+1)</f>
@@ -9354,7 +9352,7 @@
       <c r="AA53" s="22"/>
       <c r="AB53" s="22"/>
     </row>
-    <row r="54" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A54" s="29">
         <v>42430</v>
       </c>
@@ -9363,11 +9361,11 @@
       </c>
       <c r="C54" s="21" cm="1">
         <f t="array" aca="1" ref="C54" ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B54+1)</f>
-        <v>2.5084317032040518E-2</v>
+        <v>3.5003777386048776E-2</v>
       </c>
       <c r="D54" s="21" cm="1">
         <f t="array" aca="1" ref="D54" ca="1">INDIRECT("'Raw Data'!"&amp;$H$4&amp;$B54+1)</f>
-        <v>3.5003777386048776E-2</v>
+        <v>2.5084317032040518E-2</v>
       </c>
       <c r="E54" s="21" cm="1">
         <f t="array" aca="1" ref="E54" ca="1">INDIRECT("'Raw Data'!"&amp;$H$5&amp;$B54+1)</f>
@@ -9399,7 +9397,7 @@
       <c r="AA54" s="22"/>
       <c r="AB54" s="22"/>
     </row>
-    <row r="55" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A55" s="28">
         <v>42401</v>
       </c>
@@ -9408,11 +9406,11 @@
       </c>
       <c r="C55" s="21" cm="1">
         <f t="array" aca="1" ref="C55" ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B55+1)</f>
-        <v>-4.3259050115962538E-2</v>
+        <v>0.10091488771832544</v>
       </c>
       <c r="D55" s="21" cm="1">
         <f t="array" aca="1" ref="D55" ca="1">INDIRECT("'Raw Data'!"&amp;$H$4&amp;$B55+1)</f>
-        <v>0.10091488771832544</v>
+        <v>-4.3259050115962538E-2</v>
       </c>
       <c r="E55" s="21" cm="1">
         <f t="array" aca="1" ref="E55" ca="1">INDIRECT("'Raw Data'!"&amp;$H$5&amp;$B55+1)</f>
@@ -9444,7 +9442,7 @@
       <c r="AA55" s="22"/>
       <c r="AB55" s="22"/>
     </row>
-    <row r="56" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A56" s="29">
         <v>42370</v>
       </c>
@@ -9453,11 +9451,11 @@
       </c>
       <c r="C56" s="21" cm="1">
         <f t="array" aca="1" ref="C56" ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B56+1)</f>
-        <v>-0.16128213802435715</v>
+        <v>-5.1538259268998174E-2</v>
       </c>
       <c r="D56" s="21" cm="1">
         <f t="array" aca="1" ref="D56" ca="1">INDIRECT("'Raw Data'!"&amp;$H$4&amp;$B56+1)</f>
-        <v>-5.1538259268998174E-2</v>
+        <v>-0.16128213802435715</v>
       </c>
       <c r="E56" s="21" cm="1">
         <f t="array" aca="1" ref="E56" ca="1">INDIRECT("'Raw Data'!"&amp;$H$5&amp;$B56+1)</f>
@@ -9489,7 +9487,7 @@
       <c r="AA56" s="22"/>
       <c r="AB56" s="22"/>
     </row>
-    <row r="57" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A57" s="28">
         <v>42339</v>
       </c>
@@ -9498,11 +9496,11 @@
       </c>
       <c r="C57" s="21" cm="1">
         <f t="array" aca="1" ref="C57" ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B57+1)</f>
-        <v>-1.5896795672076667E-2</v>
+        <v>-8.095698405026576E-2</v>
       </c>
       <c r="D57" s="21" cm="1">
         <f t="array" aca="1" ref="D57" ca="1">INDIRECT("'Raw Data'!"&amp;$H$4&amp;$B57+1)</f>
-        <v>-8.095698405026576E-2</v>
+        <v>-1.5896795672076667E-2</v>
       </c>
       <c r="E57" s="21" cm="1">
         <f t="array" aca="1" ref="E57" ca="1">INDIRECT("'Raw Data'!"&amp;$H$5&amp;$B57+1)</f>
@@ -9534,7 +9532,7 @@
       <c r="AA57" s="22"/>
       <c r="AB57" s="22"/>
     </row>
-    <row r="58" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A58" s="29">
         <v>42309</v>
       </c>
@@ -9543,11 +9541,11 @@
       </c>
       <c r="C58" s="21" cm="1">
         <f t="array" aca="1" ref="C58" ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B58+1)</f>
-        <v>-5.9712005008608571E-2</v>
+        <v>0.15618887957530039</v>
       </c>
       <c r="D58" s="21" cm="1">
         <f t="array" aca="1" ref="D58" ca="1">INDIRECT("'Raw Data'!"&amp;$H$4&amp;$B58+1)</f>
-        <v>0.15618887957530039</v>
+        <v>-5.9712005008608571E-2</v>
       </c>
       <c r="E58" s="21" cm="1">
         <f t="array" aca="1" ref="E58" ca="1">INDIRECT("'Raw Data'!"&amp;$H$5&amp;$B58+1)</f>
@@ -9579,7 +9577,7 @@
       <c r="AA58" s="22"/>
       <c r="AB58" s="22"/>
     </row>
-    <row r="59" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A59" s="28">
         <v>42278</v>
       </c>
@@ -9588,11 +9586,11 @@
       </c>
       <c r="C59" s="21" cm="1">
         <f t="array" aca="1" ref="C59" ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B59+1)</f>
-        <v>4.3357556952723239E-2</v>
+        <v>0.4710234278668311</v>
       </c>
       <c r="D59" s="21" cm="1">
         <f t="array" aca="1" ref="D59" ca="1">INDIRECT("'Raw Data'!"&amp;$H$4&amp;$B59+1)</f>
-        <v>0.4710234278668311</v>
+        <v>4.3357556952723239E-2</v>
       </c>
       <c r="E59" s="21" cm="1">
         <f t="array" aca="1" ref="E59" ca="1">INDIRECT("'Raw Data'!"&amp;$H$5&amp;$B59+1)</f>
@@ -9624,7 +9622,7 @@
       <c r="AA59" s="22"/>
       <c r="AB59" s="22"/>
     </row>
-    <row r="60" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A60" s="29">
         <v>42248</v>
       </c>
@@ -9633,11 +9631,11 @@
       </c>
       <c r="C60" s="21" cm="1">
         <f t="array" aca="1" ref="C60" ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B60+1)</f>
-        <v>2.3055717985130602E-2</v>
+        <v>-0.32020117351215427</v>
       </c>
       <c r="D60" s="21" cm="1">
         <f t="array" aca="1" ref="D60" ca="1">INDIRECT("'Raw Data'!"&amp;$H$4&amp;$B60+1)</f>
-        <v>-0.32020117351215427</v>
+        <v>2.3055717985130602E-2</v>
       </c>
       <c r="E60" s="21" cm="1">
         <f t="array" aca="1" ref="E60" ca="1">INDIRECT("'Raw Data'!"&amp;$H$5&amp;$B60+1)</f>
@@ -9669,7 +9667,7 @@
       <c r="AA60" s="22"/>
       <c r="AB60" s="22"/>
     </row>
-    <row r="61" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A61" s="28">
         <v>42217</v>
       </c>
@@ -9678,11 +9676,11 @@
       </c>
       <c r="C61" s="21" cm="1">
         <f t="array" aca="1" ref="C61" ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B61+1)</f>
-        <v>-8.4505965126950161E-2</v>
+        <v>-0.157287497056746</v>
       </c>
       <c r="D61" s="21" cm="1">
         <f t="array" aca="1" ref="D61" ca="1">INDIRECT("'Raw Data'!"&amp;$H$4&amp;$B61+1)</f>
-        <v>-0.157287497056746</v>
+        <v>-8.4505965126950161E-2</v>
       </c>
       <c r="E61" s="21" cm="1">
         <f t="array" aca="1" ref="E61" ca="1">INDIRECT("'Raw Data'!"&amp;$H$5&amp;$B61+1)</f>
@@ -9714,7 +9712,7 @@
       <c r="AA61" s="22"/>
       <c r="AB61" s="22"/>
     </row>
-    <row r="62" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A62" s="29">
         <v>42186</v>
       </c>
@@ -9723,11 +9721,11 @@
       </c>
       <c r="C62" s="21" cm="1">
         <f t="array" aca="1" ref="C62" ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B62+1)</f>
-        <v>-0.10689160576463347</v>
+        <v>-0.29685430463576151</v>
       </c>
       <c r="D62" s="21" cm="1">
         <f t="array" aca="1" ref="D62" ca="1">INDIRECT("'Raw Data'!"&amp;$H$4&amp;$B62+1)</f>
-        <v>-0.29685430463576151</v>
+        <v>-0.10689160576463347</v>
       </c>
       <c r="E62" s="21" cm="1">
         <f t="array" aca="1" ref="E62" ca="1">INDIRECT("'Raw Data'!"&amp;$H$5&amp;$B62+1)</f>
@@ -9759,7 +9757,7 @@
       <c r="AA62" s="22"/>
       <c r="AB62" s="22"/>
     </row>
-    <row r="63" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A63" s="28">
         <v>42156</v>
       </c>
@@ -9768,11 +9766,11 @@
       </c>
       <c r="C63" s="21" cm="1">
         <f t="array" aca="1" ref="C63" ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B63+1)</f>
-        <v>-3.6395945768066422E-2</v>
+        <v>-3.5143769968051151E-2</v>
       </c>
       <c r="D63" s="21" cm="1">
         <f t="array" aca="1" ref="D63" ca="1">INDIRECT("'Raw Data'!"&amp;$H$4&amp;$B63+1)</f>
-        <v>-3.5143769968051151E-2</v>
+        <v>-3.6395945768066422E-2</v>
       </c>
       <c r="E63" s="21" cm="1">
         <f t="array" aca="1" ref="E63" ca="1">INDIRECT("'Raw Data'!"&amp;$H$5&amp;$B63+1)</f>
@@ -9804,7 +9802,7 @@
       <c r="AA63" s="22"/>
       <c r="AB63" s="22"/>
     </row>
-    <row r="64" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A64" s="29">
         <v>42125</v>
       </c>
@@ -9813,11 +9811,11 @@
       </c>
       <c r="C64" s="21" cm="1">
         <f t="array" aca="1" ref="C64" ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B64+1)</f>
-        <v>-0.12229218416036046</v>
+        <v>-4.6313223644119411E-2</v>
       </c>
       <c r="D64" s="21" cm="1">
         <f t="array" aca="1" ref="D64" ca="1">INDIRECT("'Raw Data'!"&amp;$H$4&amp;$B64+1)</f>
-        <v>-4.6313223644119411E-2</v>
+        <v>-0.12229218416036046</v>
       </c>
       <c r="E64" s="21" cm="1">
         <f t="array" aca="1" ref="E64" ca="1">INDIRECT("'Raw Data'!"&amp;$H$5&amp;$B64+1)</f>
@@ -9849,7 +9847,7 @@
       <c r="AA64" s="22"/>
       <c r="AB64" s="22"/>
     </row>
-    <row r="65" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A65" s="28">
         <v>42095</v>
       </c>
@@ -9858,11 +9856,11 @@
       </c>
       <c r="C65" s="21" cm="1">
         <f t="array" aca="1" ref="C65" ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B65+1)</f>
-        <v>-3.8491446345256565E-2</v>
+        <v>-9.1613617492388638E-2</v>
       </c>
       <c r="D65" s="21" cm="1">
         <f t="array" aca="1" ref="D65" ca="1">INDIRECT("'Raw Data'!"&amp;$H$4&amp;$B65+1)</f>
-        <v>-9.1613617492388638E-2</v>
+        <v>-3.8491446345256565E-2</v>
       </c>
       <c r="E65" s="21" cm="1">
         <f t="array" aca="1" ref="E65" ca="1">INDIRECT("'Raw Data'!"&amp;$H$5&amp;$B65+1)</f>
@@ -9894,7 +9892,7 @@
       <c r="AA65" s="22"/>
       <c r="AB65" s="22"/>
     </row>
-    <row r="66" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A66" s="29">
         <v>42064</v>
       </c>
@@ -9903,11 +9901,11 @@
       </c>
       <c r="C66" s="21" cm="1">
         <f t="array" aca="1" ref="C66" ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B66+1)</f>
-        <v>1.026878401885415E-2</v>
+        <v>-6.4232064232064207E-2</v>
       </c>
       <c r="D66" s="21" cm="1">
         <f t="array" aca="1" ref="D66" ca="1">INDIRECT("'Raw Data'!"&amp;$H$4&amp;$B66+1)</f>
-        <v>-6.4232064232064207E-2</v>
+        <v>1.026878401885415E-2</v>
       </c>
       <c r="E66" s="21" cm="1">
         <f t="array" aca="1" ref="E66" ca="1">INDIRECT("'Raw Data'!"&amp;$H$5&amp;$B66+1)</f>
@@ -9939,7 +9937,7 @@
       <c r="AA66" s="22"/>
       <c r="AB66" s="22"/>
     </row>
-    <row r="67" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A67" s="28">
         <v>42036</v>
       </c>
@@ -9948,11 +9946,11 @@
       </c>
       <c r="C67" s="21" cm="1">
         <f t="array" aca="1" ref="C67" ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B67+1)</f>
-        <v>8.9369765878109977E-2</v>
+        <v>2.9462738301559804E-2</v>
       </c>
       <c r="D67" s="21" cm="1">
         <f t="array" aca="1" ref="D67" ca="1">INDIRECT("'Raw Data'!"&amp;$H$4&amp;$B67+1)</f>
-        <v>2.9462738301559804E-2</v>
+        <v>8.9369765878109977E-2</v>
       </c>
       <c r="E67" s="21" cm="1">
         <f t="array" aca="1" ref="E67" ca="1">INDIRECT("'Raw Data'!"&amp;$H$5&amp;$B67+1)</f>
@@ -9984,7 +9982,7 @@
       <c r="AA67" s="22"/>
       <c r="AB67" s="22"/>
     </row>
-    <row r="68" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A68" s="29">
         <v>42005</v>
       </c>
@@ -9993,11 +9991,11 @@
       </c>
       <c r="C68" s="21" cm="1">
         <f t="array" aca="1" ref="C68" ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B68+1)</f>
-        <v>2.2885012192834345E-2</v>
+        <v>5.4251581166549497E-2</v>
       </c>
       <c r="D68" s="21" cm="1">
         <f t="array" aca="1" ref="D68" ca="1">INDIRECT("'Raw Data'!"&amp;$H$4&amp;$B68+1)</f>
-        <v>5.4251581166549497E-2</v>
+        <v>2.2885012192834345E-2</v>
       </c>
       <c r="E68" s="21" cm="1">
         <f t="array" aca="1" ref="E68" ca="1">INDIRECT("'Raw Data'!"&amp;$H$5&amp;$B68+1)</f>
@@ -10029,7 +10027,7 @@
       <c r="AA68" s="22"/>
       <c r="AB68" s="22"/>
     </row>
-    <row r="69" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A69" s="28">
         <v>41974</v>
       </c>
@@ -10038,11 +10036,11 @@
       </c>
       <c r="C69" s="21" cm="1">
         <f t="array" aca="1" ref="C69" ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B69+1)</f>
-        <v>-3.3188248095756226E-2</v>
+        <v>3.1907179115300971E-2</v>
       </c>
       <c r="D69" s="21" cm="1">
         <f t="array" aca="1" ref="D69" ca="1">INDIRECT("'Raw Data'!"&amp;$H$4&amp;$B69+1)</f>
-        <v>3.1907179115300971E-2</v>
+        <v>-3.3188248095756226E-2</v>
       </c>
       <c r="E69" s="21" cm="1">
         <f t="array" aca="1" ref="E69" ca="1">INDIRECT("'Raw Data'!"&amp;$H$5&amp;$B69+1)</f>
@@ -10074,7 +10072,7 @@
       <c r="AA69" s="22"/>
       <c r="AB69" s="22"/>
     </row>
-    <row r="70" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A70" s="29">
         <v>41944</v>
       </c>
@@ -10083,11 +10081,11 @@
       </c>
       <c r="C70" s="21" cm="1">
         <f t="array" aca="1" ref="C70" ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B70+1)</f>
-        <v>-0.13310973692485065</v>
+        <v>-1.175290239357888E-2</v>
       </c>
       <c r="D70" s="21" cm="1">
         <f t="array" aca="1" ref="D70" ca="1">INDIRECT("'Raw Data'!"&amp;$H$4&amp;$B70+1)</f>
-        <v>-1.175290239357888E-2</v>
+        <v>-0.13310973692485065</v>
       </c>
       <c r="E70" s="21" cm="1">
         <f t="array" aca="1" ref="E70" ca="1">INDIRECT("'Raw Data'!"&amp;$H$5&amp;$B70+1)</f>
@@ -10119,7 +10117,7 @@
       <c r="AA70" s="22"/>
       <c r="AB70" s="22"/>
     </row>
-    <row r="71" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A71" s="28">
         <v>41913</v>
       </c>
@@ -10128,11 +10126,11 @@
       </c>
       <c r="C71" s="21" cm="1">
         <f t="array" aca="1" ref="C71" ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B71+1)</f>
-        <v>-6.5798492117889101E-2</v>
+        <v>4.9646457048292507E-2</v>
       </c>
       <c r="D71" s="21" cm="1">
         <f t="array" aca="1" ref="D71" ca="1">INDIRECT("'Raw Data'!"&amp;$H$4&amp;$B71+1)</f>
-        <v>4.9646457048292507E-2</v>
+        <v>-6.5798492117889101E-2</v>
       </c>
       <c r="E71" s="21" cm="1">
         <f t="array" aca="1" ref="E71" ca="1">INDIRECT("'Raw Data'!"&amp;$H$5&amp;$B71+1)</f>
@@ -10164,7 +10162,7 @@
       <c r="AA71" s="22"/>
       <c r="AB71" s="22"/>
     </row>
-    <row r="72" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A72" s="29">
         <v>41883</v>
       </c>
@@ -10173,11 +10171,11 @@
       </c>
       <c r="C72" s="21" cm="1">
         <f t="array" aca="1" ref="C72" ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B72+1)</f>
-        <v>3.1668266074044243E-2</v>
+        <v>-2.019457547169818E-2</v>
       </c>
       <c r="D72" s="21" cm="1">
         <f t="array" aca="1" ref="D72" ca="1">INDIRECT("'Raw Data'!"&amp;$H$4&amp;$B72+1)</f>
-        <v>-2.019457547169818E-2</v>
+        <v>3.1668266074044243E-2</v>
       </c>
       <c r="E72" s="21" cm="1">
         <f t="array" aca="1" ref="E72" ca="1">INDIRECT("'Raw Data'!"&amp;$H$5&amp;$B72+1)</f>
@@ -10209,7 +10207,7 @@
       <c r="AA72" s="22"/>
       <c r="AB72" s="22"/>
     </row>
-    <row r="73" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A73" s="28">
         <v>41852</v>
       </c>
@@ -10218,11 +10216,11 @@
       </c>
       <c r="C73" s="21" cm="1">
         <f t="array" aca="1" ref="C73" ca="1">INDIRECT("'Raw Data'!"&amp;$H$3&amp;B73+1)</f>
-        <v>-1.3404424955152554E-2</v>
+        <v>8.6831143864146157E-2</v>
       </c>
       <c r="D73" s="21" cm="1">
         <f t="array" aca="1" ref="D73" ca="1">INDIRECT("'Raw Data'!"&amp;$H$4&amp;$B73+1)</f>
-        <v>8.6831143864146157E-2</v>
+        <v>-1.3404424955152554E-2</v>
       </c>
       <c r="E73" s="21" cm="1">
         <f t="array" aca="1" ref="E73" ca="1">INDIRECT("'Raw Data'!"&amp;$H$5&amp;$B73+1)</f>
@@ -10254,7 +10252,7 @@
       <c r="AA73" s="22"/>
       <c r="AB73" s="22"/>
     </row>
-    <row r="74" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A74" s="26"/>
       <c r="B74" s="27"/>
       <c r="C74" s="22"/>
@@ -10283,7 +10281,7 @@
       <c r="AA74" s="22"/>
       <c r="AB74" s="22"/>
     </row>
-    <row r="75" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A75" s="55"/>
       <c r="B75" s="55"/>
       <c r="C75" s="22"/>
@@ -10313,7 +10311,7 @@
       <c r="AA75" s="22"/>
       <c r="AB75" s="22"/>
     </row>
-    <row r="76" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A76" s="55"/>
       <c r="B76" s="55"/>
       <c r="C76" s="22"/>
@@ -10343,7 +10341,7 @@
       <c r="AA76" s="22"/>
       <c r="AB76" s="22"/>
     </row>
-    <row r="77" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A77" s="55"/>
       <c r="B77" s="55"/>
       <c r="C77" s="22"/>
@@ -10373,7 +10371,7 @@
       <c r="AA77" s="22"/>
       <c r="AB77" s="22"/>
     </row>
-    <row r="78" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A78" s="55"/>
       <c r="B78" s="55"/>
       <c r="C78" s="22"/>
@@ -10403,251 +10401,251 @@
       <c r="AA78" s="22"/>
       <c r="AB78" s="22"/>
     </row>
-    <row r="79" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
     </row>
-    <row r="80" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115" s="1"/>
       <c r="B115" s="1"/>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" s="1"/>
       <c r="B116" s="1"/>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C122" s="2"/>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C123" s="2"/>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C124" s="2"/>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C125" s="2"/>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C126" s="2"/>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C127" s="2"/>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C128" s="2"/>
     </row>
-    <row r="129" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C129" s="2"/>
     </row>
-    <row r="130" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C130" s="2"/>
     </row>
-    <row r="131" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="131" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C131" s="2"/>
     </row>
-    <row r="132" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C132" s="2"/>
     </row>
-    <row r="133" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C133" s="2"/>
     </row>
-    <row r="134" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C134" s="2"/>
     </row>
-    <row r="135" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="135" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C135" s="2"/>
     </row>
-    <row r="136" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C136" s="2"/>
     </row>
-    <row r="137" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C137" s="2"/>
     </row>
-    <row r="138" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C138" s="2"/>
     </row>
-    <row r="139" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C139" s="2"/>
     </row>
-    <row r="140" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="140" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C140" s="2"/>
     </row>
-    <row r="141" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="141" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C141" s="2"/>
     </row>
-    <row r="142" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="142" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C142" s="2"/>
     </row>
-    <row r="143" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="143" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C143" s="2"/>
     </row>
-    <row r="144" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="144" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C144" s="2"/>
     </row>
-    <row r="145" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="145" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C145" s="2"/>
     </row>
-    <row r="146" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="146" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C146" s="2"/>
     </row>
   </sheetData>
@@ -10683,25 +10681,25 @@
       <selection activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" hidden="1" customWidth="1"/>
     <col min="3" max="6" width="12" customWidth="1"/>
     <col min="8" max="8" width="0" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="29.5703125" customWidth="1"/>
-    <col min="10" max="10" width="21.85546875" customWidth="1"/>
-    <col min="11" max="11" width="14.28515625" customWidth="1"/>
-    <col min="12" max="12" width="30.5703125" customWidth="1"/>
-    <col min="13" max="13" width="11.85546875" customWidth="1"/>
-    <col min="14" max="14" width="9.140625" customWidth="1"/>
-    <col min="15" max="15" width="28.28515625" customWidth="1"/>
-    <col min="16" max="16" width="17.42578125" customWidth="1"/>
-    <col min="17" max="17" width="14.28515625" customWidth="1"/>
-    <col min="18" max="18" width="12.7109375" customWidth="1"/>
+    <col min="9" max="9" width="29.5" customWidth="1"/>
+    <col min="10" max="10" width="21.83203125" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" customWidth="1"/>
+    <col min="12" max="12" width="30.5" customWidth="1"/>
+    <col min="13" max="13" width="11.83203125" customWidth="1"/>
+    <col min="14" max="14" width="9.1640625" customWidth="1"/>
+    <col min="15" max="15" width="28.33203125" customWidth="1"/>
+    <col min="16" max="16" width="17.5" customWidth="1"/>
+    <col min="17" max="17" width="14.33203125" customWidth="1"/>
+    <col min="18" max="18" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1" s="32" t="s">
         <v>1210</v>
       </c>
@@ -10731,7 +10729,7 @@
       <c r="AA1" s="22"/>
       <c r="AB1" s="22"/>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
         <v>0</v>
       </c>
@@ -10781,7 +10779,7 @@
       <c r="AA2" s="22"/>
       <c r="AB2" s="22"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A3" s="28">
         <v>43983</v>
       </c>
@@ -10830,7 +10828,7 @@
       <c r="AA3" s="22"/>
       <c r="AB3" s="22"/>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A4" s="29">
         <v>43952</v>
       </c>
@@ -10883,7 +10881,7 @@
       <c r="AA4" s="22"/>
       <c r="AB4" s="22"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A5" s="28">
         <v>43922</v>
       </c>
@@ -10937,7 +10935,7 @@
       <c r="AA5" s="22"/>
       <c r="AB5" s="22"/>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A6" s="29">
         <v>43891</v>
       </c>
@@ -10991,7 +10989,7 @@
       <c r="AA6" s="22"/>
       <c r="AB6" s="22"/>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A7" s="28">
         <v>43862</v>
       </c>
@@ -11041,7 +11039,7 @@
       <c r="AA7" s="22"/>
       <c r="AB7" s="22"/>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A8" s="29">
         <v>43831</v>
       </c>
@@ -11091,7 +11089,7 @@
       <c r="AA8" s="22"/>
       <c r="AB8" s="22"/>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A9" s="28">
         <v>43800</v>
       </c>
@@ -11136,7 +11134,7 @@
       <c r="AA9" s="22"/>
       <c r="AB9" s="22"/>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A10" s="29">
         <v>43770</v>
       </c>
@@ -11185,7 +11183,7 @@
       <c r="AA10" s="22"/>
       <c r="AB10" s="22"/>
     </row>
-    <row r="11" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="28">
         <v>43739</v>
       </c>
@@ -11242,7 +11240,7 @@
       <c r="AA11" s="22"/>
       <c r="AB11" s="22"/>
     </row>
-    <row r="12" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="29">
         <v>43709</v>
       </c>
@@ -11299,7 +11297,7 @@
       <c r="AA12" s="22"/>
       <c r="AB12" s="22"/>
     </row>
-    <row r="13" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="28">
         <v>43678</v>
       </c>
@@ -11356,7 +11354,7 @@
       <c r="AA13" s="22"/>
       <c r="AB13" s="22"/>
     </row>
-    <row r="14" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="29">
         <v>43647</v>
       </c>
@@ -11413,7 +11411,7 @@
       <c r="AA14" s="22"/>
       <c r="AB14" s="22"/>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A15" s="28">
         <v>43617</v>
       </c>
@@ -11462,7 +11460,7 @@
       <c r="AA15" s="22"/>
       <c r="AB15" s="22"/>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A16" s="29">
         <v>43586</v>
       </c>
@@ -11516,7 +11514,7 @@
       <c r="AA16" s="22"/>
       <c r="AB16" s="22"/>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A17" s="28">
         <v>43556</v>
       </c>
@@ -11561,7 +11559,7 @@
       <c r="AA17" s="22"/>
       <c r="AB17" s="22"/>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A18" s="29">
         <v>43525</v>
       </c>
@@ -11608,7 +11606,7 @@
       <c r="AA18" s="22"/>
       <c r="AB18" s="22"/>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A19" s="28">
         <v>43497</v>
       </c>
@@ -11659,7 +11657,7 @@
       <c r="AA19" s="22"/>
       <c r="AB19" s="22"/>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A20" s="29">
         <v>43466</v>
       </c>
@@ -11714,7 +11712,7 @@
       <c r="AA20" s="22"/>
       <c r="AB20" s="22"/>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A21" s="28">
         <v>43435</v>
       </c>
@@ -11770,7 +11768,7 @@
       <c r="AA21" s="22"/>
       <c r="AB21" s="22"/>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A22" s="29">
         <v>43405</v>
       </c>
@@ -11826,7 +11824,7 @@
       <c r="AA22" s="22"/>
       <c r="AB22" s="22"/>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A23" s="28">
         <v>43374</v>
       </c>
@@ -11881,7 +11879,7 @@
       <c r="AA23" s="22"/>
       <c r="AB23" s="22"/>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A24" s="29">
         <v>43344</v>
       </c>
@@ -11923,7 +11921,7 @@
       <c r="AA24" s="22"/>
       <c r="AB24" s="22"/>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A25" s="28">
         <v>43313</v>
       </c>
@@ -11970,7 +11968,7 @@
       <c r="AA25" s="22"/>
       <c r="AB25" s="22"/>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A26" s="29">
         <v>43282</v>
       </c>
@@ -12019,7 +12017,7 @@
       <c r="AA26" s="22"/>
       <c r="AB26" s="22"/>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A27" s="28">
         <v>43252</v>
       </c>
@@ -12068,7 +12066,7 @@
       <c r="AA27" s="22"/>
       <c r="AB27" s="22"/>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A28" s="29">
         <v>43221</v>
       </c>
@@ -12113,7 +12111,7 @@
       <c r="AA28" s="22"/>
       <c r="AB28" s="22"/>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A29" s="28">
         <v>43191</v>
       </c>
@@ -12172,7 +12170,7 @@
       <c r="AA29" s="22"/>
       <c r="AB29" s="22"/>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A30" s="29">
         <v>43160</v>
       </c>
@@ -12231,7 +12229,7 @@
       <c r="AA30" s="22"/>
       <c r="AB30" s="22"/>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A31" s="28">
         <v>43132</v>
       </c>
@@ -12290,7 +12288,7 @@
       <c r="AA31" s="22"/>
       <c r="AB31" s="22"/>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A32" s="29">
         <v>43101</v>
       </c>
@@ -12349,7 +12347,7 @@
       <c r="AA32" s="22"/>
       <c r="AB32" s="22"/>
     </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A33" s="28">
         <v>43070</v>
       </c>
@@ -12408,7 +12406,7 @@
       <c r="AA33" s="22"/>
       <c r="AB33" s="22"/>
     </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A34" s="29">
         <v>43040</v>
       </c>
@@ -12453,7 +12451,7 @@
       <c r="AA34" s="22"/>
       <c r="AB34" s="22"/>
     </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A35" s="28">
         <v>43009</v>
       </c>
@@ -12500,7 +12498,7 @@
       <c r="AA35" s="22"/>
       <c r="AB35" s="22"/>
     </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A36" s="29">
         <v>42979</v>
       </c>
@@ -12547,7 +12545,7 @@
       <c r="AA36" s="22"/>
       <c r="AB36" s="22"/>
     </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A37" s="28">
         <v>42948</v>
       </c>
@@ -12594,7 +12592,7 @@
       <c r="AA37" s="22"/>
       <c r="AB37" s="22"/>
     </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A38" s="29">
         <v>42917</v>
       </c>
@@ -12641,7 +12639,7 @@
       <c r="AA38" s="22"/>
       <c r="AB38" s="22"/>
     </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A39" s="28">
         <v>42887</v>
       </c>
@@ -12688,7 +12686,7 @@
       <c r="AA39" s="22"/>
       <c r="AB39" s="22"/>
     </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A40" s="29">
         <v>42856</v>
       </c>
@@ -12735,7 +12733,7 @@
       <c r="AA40" s="22"/>
       <c r="AB40" s="22"/>
     </row>
-    <row r="41" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A41" s="28">
         <v>42826</v>
       </c>
@@ -12780,7 +12778,7 @@
       <c r="AA41" s="22"/>
       <c r="AB41" s="22"/>
     </row>
-    <row r="42" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A42" s="29">
         <v>42795</v>
       </c>
@@ -12827,7 +12825,7 @@
       <c r="AA42" s="22"/>
       <c r="AB42" s="22"/>
     </row>
-    <row r="43" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A43" s="28">
         <v>42767</v>
       </c>
@@ -12872,7 +12870,7 @@
       <c r="AA43" s="22"/>
       <c r="AB43" s="22"/>
     </row>
-    <row r="44" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A44" s="29">
         <v>42736</v>
       </c>
@@ -12917,7 +12915,7 @@
       <c r="AA44" s="22"/>
       <c r="AB44" s="22"/>
     </row>
-    <row r="45" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A45" s="28">
         <v>42705</v>
       </c>
@@ -12962,7 +12960,7 @@
       <c r="AA45" s="22"/>
       <c r="AB45" s="22"/>
     </row>
-    <row r="46" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A46" s="29">
         <v>42675</v>
       </c>
@@ -13007,7 +13005,7 @@
       <c r="AA46" s="22"/>
       <c r="AB46" s="22"/>
     </row>
-    <row r="47" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A47" s="28">
         <v>42644</v>
       </c>
@@ -13052,7 +13050,7 @@
       <c r="AA47" s="22"/>
       <c r="AB47" s="22"/>
     </row>
-    <row r="48" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A48" s="29">
         <v>42614</v>
       </c>
@@ -13097,7 +13095,7 @@
       <c r="AA48" s="22"/>
       <c r="AB48" s="22"/>
     </row>
-    <row r="49" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A49" s="28">
         <v>42583</v>
       </c>
@@ -13142,7 +13140,7 @@
       <c r="AA49" s="22"/>
       <c r="AB49" s="22"/>
     </row>
-    <row r="50" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A50" s="29">
         <v>42552</v>
       </c>
@@ -13187,7 +13185,7 @@
       <c r="AA50" s="22"/>
       <c r="AB50" s="22"/>
     </row>
-    <row r="51" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A51" s="28">
         <v>42522</v>
       </c>
@@ -13232,7 +13230,7 @@
       <c r="AA51" s="22"/>
       <c r="AB51" s="22"/>
     </row>
-    <row r="52" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A52" s="29">
         <v>42491</v>
       </c>
@@ -13277,7 +13275,7 @@
       <c r="AA52" s="22"/>
       <c r="AB52" s="22"/>
     </row>
-    <row r="53" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A53" s="28">
         <v>42461</v>
       </c>
@@ -13322,7 +13320,7 @@
       <c r="AA53" s="22"/>
       <c r="AB53" s="22"/>
     </row>
-    <row r="54" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A54" s="29">
         <v>42430</v>
       </c>
@@ -13367,7 +13365,7 @@
       <c r="AA54" s="22"/>
       <c r="AB54" s="22"/>
     </row>
-    <row r="55" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A55" s="28">
         <v>42401</v>
       </c>
@@ -13412,7 +13410,7 @@
       <c r="AA55" s="22"/>
       <c r="AB55" s="22"/>
     </row>
-    <row r="56" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A56" s="29">
         <v>42370</v>
       </c>
@@ -13457,7 +13455,7 @@
       <c r="AA56" s="22"/>
       <c r="AB56" s="22"/>
     </row>
-    <row r="57" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A57" s="28">
         <v>42339</v>
       </c>
@@ -13502,7 +13500,7 @@
       <c r="AA57" s="22"/>
       <c r="AB57" s="22"/>
     </row>
-    <row r="58" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A58" s="29">
         <v>42309</v>
       </c>
@@ -13547,7 +13545,7 @@
       <c r="AA58" s="22"/>
       <c r="AB58" s="22"/>
     </row>
-    <row r="59" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A59" s="28">
         <v>42278</v>
       </c>
@@ -13592,7 +13590,7 @@
       <c r="AA59" s="22"/>
       <c r="AB59" s="22"/>
     </row>
-    <row r="60" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A60" s="29">
         <v>42248</v>
       </c>
@@ -13637,7 +13635,7 @@
       <c r="AA60" s="22"/>
       <c r="AB60" s="22"/>
     </row>
-    <row r="61" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A61" s="28">
         <v>42217</v>
       </c>
@@ -13682,7 +13680,7 @@
       <c r="AA61" s="22"/>
       <c r="AB61" s="22"/>
     </row>
-    <row r="62" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A62" s="29">
         <v>42186</v>
       </c>
@@ -13727,7 +13725,7 @@
       <c r="AA62" s="22"/>
       <c r="AB62" s="22"/>
     </row>
-    <row r="63" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A63" s="28">
         <v>42156</v>
       </c>
@@ -13772,7 +13770,7 @@
       <c r="AA63" s="22"/>
       <c r="AB63" s="22"/>
     </row>
-    <row r="64" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A64" s="29">
         <v>42125</v>
       </c>
@@ -13817,7 +13815,7 @@
       <c r="AA64" s="22"/>
       <c r="AB64" s="22"/>
     </row>
-    <row r="65" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A65" s="28">
         <v>42095</v>
       </c>
@@ -13862,7 +13860,7 @@
       <c r="AA65" s="22"/>
       <c r="AB65" s="22"/>
     </row>
-    <row r="66" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A66" s="29">
         <v>42064</v>
       </c>
@@ -13907,7 +13905,7 @@
       <c r="AA66" s="22"/>
       <c r="AB66" s="22"/>
     </row>
-    <row r="67" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A67" s="28">
         <v>42036</v>
       </c>
@@ -13952,7 +13950,7 @@
       <c r="AA67" s="22"/>
       <c r="AB67" s="22"/>
     </row>
-    <row r="68" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A68" s="29">
         <v>42005</v>
       </c>
@@ -13997,7 +13995,7 @@
       <c r="AA68" s="22"/>
       <c r="AB68" s="22"/>
     </row>
-    <row r="69" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A69" s="28">
         <v>41974</v>
       </c>
@@ -14042,7 +14040,7 @@
       <c r="AA69" s="22"/>
       <c r="AB69" s="22"/>
     </row>
-    <row r="70" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A70" s="29">
         <v>41944</v>
       </c>
@@ -14087,7 +14085,7 @@
       <c r="AA70" s="22"/>
       <c r="AB70" s="22"/>
     </row>
-    <row r="71" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A71" s="28">
         <v>41913</v>
       </c>
@@ -14132,7 +14130,7 @@
       <c r="AA71" s="22"/>
       <c r="AB71" s="22"/>
     </row>
-    <row r="72" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A72" s="29">
         <v>41883</v>
       </c>
@@ -14177,7 +14175,7 @@
       <c r="AA72" s="22"/>
       <c r="AB72" s="22"/>
     </row>
-    <row r="73" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A73" s="28">
         <v>41852</v>
       </c>
@@ -14222,7 +14220,7 @@
       <c r="AA73" s="22"/>
       <c r="AB73" s="22"/>
     </row>
-    <row r="74" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A74" s="26"/>
       <c r="B74" s="27"/>
       <c r="C74" s="22"/>
@@ -14251,7 +14249,7 @@
       <c r="AA74" s="22"/>
       <c r="AB74" s="22"/>
     </row>
-    <row r="75" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A75" s="55"/>
       <c r="B75" s="55"/>
       <c r="C75" s="22"/>
@@ -14281,7 +14279,7 @@
       <c r="AA75" s="22"/>
       <c r="AB75" s="22"/>
     </row>
-    <row r="76" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A76" s="55"/>
       <c r="B76" s="55"/>
       <c r="C76" s="22"/>
@@ -14311,7 +14309,7 @@
       <c r="AA76" s="22"/>
       <c r="AB76" s="22"/>
     </row>
-    <row r="77" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A77" s="55"/>
       <c r="B77" s="55"/>
       <c r="C77" s="22"/>
@@ -14341,7 +14339,7 @@
       <c r="AA77" s="22"/>
       <c r="AB77" s="22"/>
     </row>
-    <row r="78" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A78" s="55"/>
       <c r="B78" s="55"/>
       <c r="C78" s="22"/>
@@ -14371,251 +14369,251 @@
       <c r="AA78" s="22"/>
       <c r="AB78" s="22"/>
     </row>
-    <row r="79" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
     </row>
-    <row r="80" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115" s="1"/>
       <c r="B115" s="1"/>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" s="1"/>
       <c r="B116" s="1"/>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C122" s="2"/>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C123" s="2"/>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C124" s="2"/>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C125" s="2"/>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C126" s="2"/>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C127" s="2"/>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C128" s="2"/>
     </row>
-    <row r="129" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C129" s="2"/>
     </row>
-    <row r="130" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C130" s="2"/>
     </row>
-    <row r="131" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="131" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C131" s="2"/>
     </row>
-    <row r="132" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C132" s="2"/>
     </row>
-    <row r="133" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C133" s="2"/>
     </row>
-    <row r="134" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C134" s="2"/>
     </row>
-    <row r="135" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="135" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C135" s="2"/>
     </row>
-    <row r="136" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C136" s="2"/>
     </row>
-    <row r="137" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C137" s="2"/>
     </row>
-    <row r="138" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C138" s="2"/>
     </row>
-    <row r="139" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C139" s="2"/>
     </row>
-    <row r="140" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="140" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C140" s="2"/>
     </row>
-    <row r="141" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="141" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C141" s="2"/>
     </row>
-    <row r="142" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="142" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C142" s="2"/>
     </row>
-    <row r="143" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="143" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C143" s="2"/>
     </row>
-    <row r="144" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="144" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C144" s="2"/>
     </row>
-    <row r="145" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="145" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C145" s="2"/>
     </row>
-    <row r="146" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="146" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C146" s="2"/>
     </row>
   </sheetData>
@@ -14651,12 +14649,12 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" customWidth="1"/>
+    <col min="1" max="1" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>19</v>
       </c>
@@ -14664,7 +14662,7 @@
         <v>1214</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>1645</v>
       </c>
@@ -14672,7 +14670,7 @@
         <v>1209</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="18" t="s">
         <v>1640</v>
       </c>
@@ -14680,7 +14678,7 @@
         <v>1644</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
         <v>1371</v>
       </c>
@@ -14688,7 +14686,7 @@
         <v>1643</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="18" t="s">
         <v>1641</v>
       </c>
@@ -14696,7 +14694,7 @@
         <v>1642</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>1646</v>
       </c>
@@ -14704,7 +14702,7 @@
         <v>1213</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>1647</v>
       </c>
@@ -14712,7 +14710,7 @@
         <v>1215</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
         <v>1208</v>
       </c>
@@ -14738,20 +14736,20 @@
       <selection activeCell="BS1" sqref="BS1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" customWidth="1"/>
-    <col min="17" max="17" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" customWidth="1"/>
+    <col min="17" max="17" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -14945,7 +14943,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="2" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>43983</v>
       </c>
@@ -15147,7 +15145,7 @@
         <v>2.7999999999999994E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>43952</v>
       </c>
@@ -15349,7 +15347,7 @@
         <v>-9.2470277410832604E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>43922</v>
       </c>
@@ -15551,7 +15549,7 @@
         <v>1.6107382550335586E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>43891</v>
       </c>
@@ -15753,7 +15751,7 @@
         <v>-0.11520190023752966</v>
       </c>
     </row>
-    <row r="6" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>43862</v>
       </c>
@@ -15955,7 +15953,7 @@
         <v>-1.1862396204032962E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>43831</v>
       </c>
@@ -16157,7 +16155,7 @@
         <v>-2.4305555555555653E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>43800</v>
       </c>
@@ -16359,7 +16357,7 @@
         <v>1.2895662368112687E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>43770</v>
       </c>
@@ -16561,7 +16559,7 @@
         <v>-8.1395348837209631E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>43739</v>
       </c>
@@ -16763,7 +16761,7 @@
         <v>3.9903264812575584E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>43709</v>
       </c>
@@ -16965,7 +16963,7 @@
         <v>-2.1301775147928963E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>43678</v>
       </c>
@@ -17167,7 +17165,7 @@
         <v>4.7562425683708859E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>43647</v>
       </c>
@@ -17369,7 +17367,7 @@
         <v>-2.5492468134414904E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>43617</v>
       </c>
@@ -17571,7 +17569,7 @@
         <v>2.0094562647754128E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>43586</v>
       </c>
@@ -17773,7 +17771,7 @@
         <v>-2.5345622119815538E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>43556</v>
       </c>
@@ -17975,7 +17973,7 @@
         <v>-2.2988505747125951E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>43525</v>
       </c>
@@ -18177,7 +18175,7 @@
         <v>-2.6845637583892641E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>43497</v>
       </c>
@@ -18379,7 +18377,7 @@
         <v>-1.1173184357541662E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>43466</v>
       </c>
@@ -18581,7 +18579,7 @@
         <v>3.3632286995514977E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>43435</v>
       </c>
@@ -18783,7 +18781,7 @@
         <v>1.2485811577752489E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>43405</v>
       </c>
@@ -18985,7 +18983,7 @@
         <v>-1.1223344556677849E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>43374</v>
       </c>
@@ -19187,7 +19185,7 @@
         <v>-4.4692737430166649E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>43344</v>
       </c>
@@ -19389,7 +19387,7 @@
         <v>-1.7563117453347987E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>43313</v>
       </c>
@@ -19591,7 +19589,7 @@
         <v>1.5607580824971993E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>43282</v>
       </c>
@@ -19793,7 +19791,7 @@
         <v>0.12547051442910928</v>
       </c>
     </row>
-    <row r="26" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>43252</v>
       </c>
@@ -19995,7 +19993,7 @@
         <v>-5.9031877213695495E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>43221</v>
       </c>
@@ -20197,7 +20195,7 @@
         <v>-0.11215932914046108</v>
       </c>
     </row>
-    <row r="28" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>43191</v>
       </c>
@@ -20399,7 +20397,7 @@
         <v>1.7057569296375089E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>43160</v>
       </c>
@@ -20601,7 +20599,7 @@
         <v>1.2958963282937472E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>43132</v>
       </c>
@@ -20803,7 +20801,7 @@
         <v>3.5794183445190191E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>43101</v>
       </c>
@@ -21005,7 +21003,7 @@
         <v>3.1141868512110676E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>43070</v>
       </c>
@@ -21207,7 +21205,7 @@
         <v>5.8608058608058664E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>43040</v>
       </c>
@@ -21409,7 +21407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>43009</v>
       </c>
@@ -21611,7 +21609,7 @@
         <v>-6.0679611650486295E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>42979</v>
       </c>
@@ -21813,7 +21811,7 @@
         <v>7.3349633251834348E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>42948</v>
       </c>
@@ -22015,7 +22013,7 @@
         <v>-8.4848484848485187E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>42917</v>
       </c>
@@ -22217,7 +22215,7 @@
         <v>-8.4134615384615728E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>42887</v>
       </c>
@@ -22419,7 +22417,7 @@
         <v>4.3914680050188275E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>42856</v>
       </c>
@@ -22621,7 +22619,7 @@
         <v>-1.4833127317676156E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>42826</v>
       </c>
@@ -22823,7 +22821,7 @@
         <v>7.436918990703846E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>42795</v>
       </c>
@@ -23025,7 +23023,7 @@
         <v>3.7190082644628163E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>42767</v>
       </c>
@@ -23227,7 +23225,7 @@
         <v>4.6109510086455245E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>42736</v>
       </c>
@@ -23429,7 +23427,7 @@
         <v>1.4430014430015404E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>42705</v>
       </c>
@@ -23631,7 +23629,7 @@
         <v>5.6402439024390266E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>42675</v>
       </c>
@@ -23833,7 +23831,7 @@
         <v>-1.649175412293858E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>42644</v>
       </c>
@@ -24035,7 +24033,7 @@
         <v>8.1037277147487846E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>42614</v>
       </c>
@@ -24237,7 +24235,7 @@
         <v>-5.6574923547400631E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>42583</v>
       </c>
@@ -24439,7 +24437,7 @@
         <v>-9.0909090909090315E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>42552</v>
       </c>
@@ -24641,7 +24639,7 @@
         <v>-1.4925373134328438E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>42522</v>
       </c>
@@ -24843,7 +24841,7 @@
         <v>3.2357473035439129E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>42491</v>
       </c>
@@ -25045,7 +25043,7 @@
         <v>-8.5915492957746406E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>42461</v>
       </c>
@@ -25247,7 +25245,7 @@
         <v>-9.762900976290137E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>42430</v>
       </c>
@@ -25449,7 +25447,7 @@
         <v>6.0650887573964522E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>42401</v>
       </c>
@@ -25651,7 +25649,7 @@
         <v>-8.7976539589443535E-3</v>
       </c>
     </row>
-    <row r="55" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>42370</v>
       </c>
@@ -25853,7 +25851,7 @@
         <v>2.0958083832335415E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>42339</v>
       </c>
@@ -26055,7 +26053,7 @@
         <v>1.0590015128592948E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>42309</v>
       </c>
@@ -26257,7 +26255,7 @@
         <v>3.6050156739811982E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>42278</v>
       </c>
@@ -26459,7 +26457,7 @@
         <v>-3.6253776435045348E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>42248</v>
       </c>
@@ -26661,7 +26659,7 @@
         <v>-2.2156573116691208E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>42217</v>
       </c>
@@ -26863,7 +26861,7 @@
         <v>-4.7819971870604883E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>42186</v>
       </c>
@@ -27065,7 +27063,7 @@
         <v>7.08215297450435E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>42156</v>
       </c>
@@ -27267,7 +27265,7 @@
         <v>1.1461318051575813E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>42125</v>
       </c>
@@ -27469,7 +27467,7 @@
         <v>1.6011644832605577E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>42095</v>
       </c>
@@ -27671,7 +27669,7 @@
         <v>-1.29310344827586E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>42064</v>
       </c>
@@ -27873,7 +27871,7 @@
         <v>1.4577259475218606E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>42036</v>
       </c>
@@ -28075,7 +28073,7 @@
         <v>5.3763440860215138E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>42005</v>
       </c>
@@ -28277,7 +28275,7 @@
         <v>-4.824561403508773E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>41974</v>
       </c>
@@ -28479,7 +28477,7 @@
         <v>-3.1161473087818664E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>41944</v>
       </c>
@@ -28681,7 +28679,7 @@
         <v>-2.4861878453038756E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>41913</v>
       </c>
@@ -28883,7 +28881,7 @@
         <v>-1.3793103448275568E-3</v>
       </c>
     </row>
-    <row r="71" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>41883</v>
       </c>
@@ -29085,7 +29083,7 @@
         <v>-1.4945652173913086E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>41852</v>
       </c>
@@ -29287,7 +29285,7 @@
         <v>2.222222222222224E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>41821</v>
       </c>

</xml_diff>

<commit_message>
Update Excel Solver Portfolio Optimization.xlsx
</commit_message>
<xml_diff>
--- a/Excel Solver Portfolio Optimization.xlsx
+++ b/Excel Solver Portfolio Optimization.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manfyegoh/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manfye\Documents\GitHub\Excel-Portfolio-Optimizer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D0DF913-B149-B743-A4E2-94221F6376DA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47CB718D-BD47-46CE-9372-79F2FEB31CD7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stock Portfolio (MPT)" sheetId="4" r:id="rId1"/>
@@ -111,7 +111,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -175,14 +177,14 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -197,7 +199,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3196" uniqueCount="1660">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3197" uniqueCount="1661">
   <si>
     <t>Date</t>
   </si>
@@ -5177,6 +5179,9 @@
   </si>
   <si>
     <t>*Solver: LP Solver</t>
+  </si>
+  <si>
+    <t>w</t>
   </si>
 </sst>
 </file>
@@ -5985,7 +5990,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="16" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="11" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
     <cellStyle name="Title" xfId="2" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="18" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="15" builtinId="11" customBuiltin="1"/>
@@ -6710,28 +6715,28 @@
   <dimension ref="A1:AB146"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" hidden="1" customWidth="1"/>
     <col min="3" max="6" width="12" customWidth="1"/>
-    <col min="8" max="8" width="8.83203125" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="29.5" customWidth="1"/>
-    <col min="10" max="10" width="21.83203125" customWidth="1"/>
-    <col min="11" max="11" width="14.33203125" customWidth="1"/>
-    <col min="12" max="12" width="30.5" customWidth="1"/>
-    <col min="13" max="13" width="11.83203125" customWidth="1"/>
-    <col min="14" max="14" width="9.1640625" customWidth="1"/>
-    <col min="15" max="15" width="28.33203125" customWidth="1"/>
-    <col min="16" max="16" width="17.5" customWidth="1"/>
-    <col min="17" max="17" width="14.33203125" customWidth="1"/>
-    <col min="18" max="18" width="12.6640625" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="29.42578125" customWidth="1"/>
+    <col min="10" max="10" width="21.85546875" customWidth="1"/>
+    <col min="11" max="11" width="14.28515625" customWidth="1"/>
+    <col min="12" max="12" width="30.42578125" customWidth="1"/>
+    <col min="13" max="13" width="11.85546875" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" customWidth="1"/>
+    <col min="15" max="15" width="28.28515625" customWidth="1"/>
+    <col min="16" max="16" width="17.42578125" customWidth="1"/>
+    <col min="17" max="17" width="14.28515625" customWidth="1"/>
+    <col min="18" max="18" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="32" t="s">
         <v>1210</v>
       </c>
@@ -6761,7 +6766,7 @@
       <c r="AA1" s="22"/>
       <c r="AB1" s="22"/>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>0</v>
       </c>
@@ -6811,7 +6816,7 @@
       <c r="AA2" s="22"/>
       <c r="AB2" s="22"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="28">
         <v>43983</v>
       </c>
@@ -6860,7 +6865,7 @@
       <c r="AA3" s="22"/>
       <c r="AB3" s="22"/>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="29">
         <v>43952</v>
       </c>
@@ -6913,7 +6918,7 @@
       <c r="AA4" s="22"/>
       <c r="AB4" s="22"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="28">
         <v>43922</v>
       </c>
@@ -6967,7 +6972,7 @@
       <c r="AA5" s="22"/>
       <c r="AB5" s="22"/>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="29">
         <v>43891</v>
       </c>
@@ -7021,7 +7026,7 @@
       <c r="AA6" s="22"/>
       <c r="AB6" s="22"/>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="28">
         <v>43862</v>
       </c>
@@ -7071,7 +7076,7 @@
       <c r="AA7" s="22"/>
       <c r="AB7" s="22"/>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" s="29">
         <v>43831</v>
       </c>
@@ -7103,7 +7108,9 @@
         <v>4.895183175195332E-2</v>
       </c>
       <c r="K8" s="22"/>
-      <c r="L8" s="22"/>
+      <c r="L8" s="22" t="s">
+        <v>1660</v>
+      </c>
       <c r="M8" s="22"/>
       <c r="N8" s="22"/>
       <c r="O8" s="22"/>
@@ -7121,7 +7128,7 @@
       <c r="AA8" s="22"/>
       <c r="AB8" s="22"/>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" s="28">
         <v>43800</v>
       </c>
@@ -7166,7 +7173,7 @@
       <c r="AA9" s="22"/>
       <c r="AB9" s="22"/>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" s="29">
         <v>43770</v>
       </c>
@@ -7215,7 +7222,7 @@
       <c r="AA10" s="22"/>
       <c r="AB10" s="22"/>
     </row>
-    <row r="11" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="28">
         <v>43739</v>
       </c>
@@ -7272,7 +7279,7 @@
       <c r="AA11" s="22"/>
       <c r="AB11" s="22"/>
     </row>
-    <row r="12" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="29">
         <v>43709</v>
       </c>
@@ -7329,7 +7336,7 @@
       <c r="AA12" s="22"/>
       <c r="AB12" s="22"/>
     </row>
-    <row r="13" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="28">
         <v>43678</v>
       </c>
@@ -7386,7 +7393,7 @@
       <c r="AA13" s="22"/>
       <c r="AB13" s="22"/>
     </row>
-    <row r="14" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="29">
         <v>43647</v>
       </c>
@@ -7443,7 +7450,7 @@
       <c r="AA14" s="22"/>
       <c r="AB14" s="22"/>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15" s="28">
         <v>43617</v>
       </c>
@@ -7492,7 +7499,7 @@
       <c r="AA15" s="22"/>
       <c r="AB15" s="22"/>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16" s="29">
         <v>43586</v>
       </c>
@@ -7546,7 +7553,7 @@
       <c r="AA16" s="22"/>
       <c r="AB16" s="22"/>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17" s="28">
         <v>43556</v>
       </c>
@@ -7591,7 +7598,7 @@
       <c r="AA17" s="22"/>
       <c r="AB17" s="22"/>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18" s="29">
         <v>43525</v>
       </c>
@@ -7638,7 +7645,7 @@
       <c r="AA18" s="22"/>
       <c r="AB18" s="22"/>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19" s="28">
         <v>43497</v>
       </c>
@@ -7689,7 +7696,7 @@
       <c r="AA19" s="22"/>
       <c r="AB19" s="22"/>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20" s="29">
         <v>43466</v>
       </c>
@@ -7744,7 +7751,7 @@
       <c r="AA20" s="22"/>
       <c r="AB20" s="22"/>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21" s="28">
         <v>43435</v>
       </c>
@@ -7800,7 +7807,7 @@
       <c r="AA21" s="22"/>
       <c r="AB21" s="22"/>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22" s="29">
         <v>43405</v>
       </c>
@@ -7856,7 +7863,7 @@
       <c r="AA22" s="22"/>
       <c r="AB22" s="22"/>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A23" s="28">
         <v>43374</v>
       </c>
@@ -7911,7 +7918,7 @@
       <c r="AA23" s="22"/>
       <c r="AB23" s="22"/>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A24" s="29">
         <v>43344</v>
       </c>
@@ -7953,7 +7960,7 @@
       <c r="AA24" s="22"/>
       <c r="AB24" s="22"/>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A25" s="28">
         <v>43313</v>
       </c>
@@ -8000,7 +8007,7 @@
       <c r="AA25" s="22"/>
       <c r="AB25" s="22"/>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A26" s="29">
         <v>43282</v>
       </c>
@@ -8049,7 +8056,7 @@
       <c r="AA26" s="22"/>
       <c r="AB26" s="22"/>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A27" s="28">
         <v>43252</v>
       </c>
@@ -8098,7 +8105,7 @@
       <c r="AA27" s="22"/>
       <c r="AB27" s="22"/>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A28" s="29">
         <v>43221</v>
       </c>
@@ -8143,7 +8150,7 @@
       <c r="AA28" s="22"/>
       <c r="AB28" s="22"/>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A29" s="28">
         <v>43191</v>
       </c>
@@ -8202,7 +8209,7 @@
       <c r="AA29" s="22"/>
       <c r="AB29" s="22"/>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A30" s="29">
         <v>43160</v>
       </c>
@@ -8261,7 +8268,7 @@
       <c r="AA30" s="22"/>
       <c r="AB30" s="22"/>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A31" s="28">
         <v>43132</v>
       </c>
@@ -8320,7 +8327,7 @@
       <c r="AA31" s="22"/>
       <c r="AB31" s="22"/>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A32" s="29">
         <v>43101</v>
       </c>
@@ -8379,7 +8386,7 @@
       <c r="AA32" s="22"/>
       <c r="AB32" s="22"/>
     </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A33" s="28">
         <v>43070</v>
       </c>
@@ -8438,7 +8445,7 @@
       <c r="AA33" s="22"/>
       <c r="AB33" s="22"/>
     </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A34" s="29">
         <v>43040</v>
       </c>
@@ -8483,7 +8490,7 @@
       <c r="AA34" s="22"/>
       <c r="AB34" s="22"/>
     </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A35" s="28">
         <v>43009</v>
       </c>
@@ -8530,7 +8537,7 @@
       <c r="AA35" s="22"/>
       <c r="AB35" s="22"/>
     </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A36" s="29">
         <v>42979</v>
       </c>
@@ -8577,7 +8584,7 @@
       <c r="AA36" s="22"/>
       <c r="AB36" s="22"/>
     </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A37" s="28">
         <v>42948</v>
       </c>
@@ -8624,7 +8631,7 @@
       <c r="AA37" s="22"/>
       <c r="AB37" s="22"/>
     </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A38" s="29">
         <v>42917</v>
       </c>
@@ -8671,7 +8678,7 @@
       <c r="AA38" s="22"/>
       <c r="AB38" s="22"/>
     </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A39" s="28">
         <v>42887</v>
       </c>
@@ -8718,7 +8725,7 @@
       <c r="AA39" s="22"/>
       <c r="AB39" s="22"/>
     </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A40" s="29">
         <v>42856</v>
       </c>
@@ -8765,7 +8772,7 @@
       <c r="AA40" s="22"/>
       <c r="AB40" s="22"/>
     </row>
-    <row r="41" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A41" s="28">
         <v>42826</v>
       </c>
@@ -8810,7 +8817,7 @@
       <c r="AA41" s="22"/>
       <c r="AB41" s="22"/>
     </row>
-    <row r="42" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A42" s="29">
         <v>42795</v>
       </c>
@@ -8857,7 +8864,7 @@
       <c r="AA42" s="22"/>
       <c r="AB42" s="22"/>
     </row>
-    <row r="43" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A43" s="28">
         <v>42767</v>
       </c>
@@ -8902,7 +8909,7 @@
       <c r="AA43" s="22"/>
       <c r="AB43" s="22"/>
     </row>
-    <row r="44" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A44" s="29">
         <v>42736</v>
       </c>
@@ -8947,7 +8954,7 @@
       <c r="AA44" s="22"/>
       <c r="AB44" s="22"/>
     </row>
-    <row r="45" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A45" s="28">
         <v>42705</v>
       </c>
@@ -8992,7 +8999,7 @@
       <c r="AA45" s="22"/>
       <c r="AB45" s="22"/>
     </row>
-    <row r="46" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A46" s="29">
         <v>42675</v>
       </c>
@@ -9037,7 +9044,7 @@
       <c r="AA46" s="22"/>
       <c r="AB46" s="22"/>
     </row>
-    <row r="47" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A47" s="28">
         <v>42644</v>
       </c>
@@ -9082,7 +9089,7 @@
       <c r="AA47" s="22"/>
       <c r="AB47" s="22"/>
     </row>
-    <row r="48" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A48" s="29">
         <v>42614</v>
       </c>
@@ -9127,7 +9134,7 @@
       <c r="AA48" s="22"/>
       <c r="AB48" s="22"/>
     </row>
-    <row r="49" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A49" s="28">
         <v>42583</v>
       </c>
@@ -9172,7 +9179,7 @@
       <c r="AA49" s="22"/>
       <c r="AB49" s="22"/>
     </row>
-    <row r="50" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A50" s="29">
         <v>42552</v>
       </c>
@@ -9217,7 +9224,7 @@
       <c r="AA50" s="22"/>
       <c r="AB50" s="22"/>
     </row>
-    <row r="51" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A51" s="28">
         <v>42522</v>
       </c>
@@ -9262,7 +9269,7 @@
       <c r="AA51" s="22"/>
       <c r="AB51" s="22"/>
     </row>
-    <row r="52" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A52" s="29">
         <v>42491</v>
       </c>
@@ -9307,7 +9314,7 @@
       <c r="AA52" s="22"/>
       <c r="AB52" s="22"/>
     </row>
-    <row r="53" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A53" s="28">
         <v>42461</v>
       </c>
@@ -9352,7 +9359,7 @@
       <c r="AA53" s="22"/>
       <c r="AB53" s="22"/>
     </row>
-    <row r="54" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A54" s="29">
         <v>42430</v>
       </c>
@@ -9397,7 +9404,7 @@
       <c r="AA54" s="22"/>
       <c r="AB54" s="22"/>
     </row>
-    <row r="55" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A55" s="28">
         <v>42401</v>
       </c>
@@ -9442,7 +9449,7 @@
       <c r="AA55" s="22"/>
       <c r="AB55" s="22"/>
     </row>
-    <row r="56" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A56" s="29">
         <v>42370</v>
       </c>
@@ -9487,7 +9494,7 @@
       <c r="AA56" s="22"/>
       <c r="AB56" s="22"/>
     </row>
-    <row r="57" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A57" s="28">
         <v>42339</v>
       </c>
@@ -9532,7 +9539,7 @@
       <c r="AA57" s="22"/>
       <c r="AB57" s="22"/>
     </row>
-    <row r="58" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A58" s="29">
         <v>42309</v>
       </c>
@@ -9577,7 +9584,7 @@
       <c r="AA58" s="22"/>
       <c r="AB58" s="22"/>
     </row>
-    <row r="59" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A59" s="28">
         <v>42278</v>
       </c>
@@ -9622,7 +9629,7 @@
       <c r="AA59" s="22"/>
       <c r="AB59" s="22"/>
     </row>
-    <row r="60" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A60" s="29">
         <v>42248</v>
       </c>
@@ -9667,7 +9674,7 @@
       <c r="AA60" s="22"/>
       <c r="AB60" s="22"/>
     </row>
-    <row r="61" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A61" s="28">
         <v>42217</v>
       </c>
@@ -9712,7 +9719,7 @@
       <c r="AA61" s="22"/>
       <c r="AB61" s="22"/>
     </row>
-    <row r="62" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A62" s="29">
         <v>42186</v>
       </c>
@@ -9757,7 +9764,7 @@
       <c r="AA62" s="22"/>
       <c r="AB62" s="22"/>
     </row>
-    <row r="63" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A63" s="28">
         <v>42156</v>
       </c>
@@ -9802,7 +9809,7 @@
       <c r="AA63" s="22"/>
       <c r="AB63" s="22"/>
     </row>
-    <row r="64" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A64" s="29">
         <v>42125</v>
       </c>
@@ -9847,7 +9854,7 @@
       <c r="AA64" s="22"/>
       <c r="AB64" s="22"/>
     </row>
-    <row r="65" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A65" s="28">
         <v>42095</v>
       </c>
@@ -9892,7 +9899,7 @@
       <c r="AA65" s="22"/>
       <c r="AB65" s="22"/>
     </row>
-    <row r="66" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A66" s="29">
         <v>42064</v>
       </c>
@@ -9937,7 +9944,7 @@
       <c r="AA66" s="22"/>
       <c r="AB66" s="22"/>
     </row>
-    <row r="67" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A67" s="28">
         <v>42036</v>
       </c>
@@ -9982,7 +9989,7 @@
       <c r="AA67" s="22"/>
       <c r="AB67" s="22"/>
     </row>
-    <row r="68" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A68" s="29">
         <v>42005</v>
       </c>
@@ -10027,7 +10034,7 @@
       <c r="AA68" s="22"/>
       <c r="AB68" s="22"/>
     </row>
-    <row r="69" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A69" s="28">
         <v>41974</v>
       </c>
@@ -10072,7 +10079,7 @@
       <c r="AA69" s="22"/>
       <c r="AB69" s="22"/>
     </row>
-    <row r="70" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A70" s="29">
         <v>41944</v>
       </c>
@@ -10117,7 +10124,7 @@
       <c r="AA70" s="22"/>
       <c r="AB70" s="22"/>
     </row>
-    <row r="71" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A71" s="28">
         <v>41913</v>
       </c>
@@ -10162,7 +10169,7 @@
       <c r="AA71" s="22"/>
       <c r="AB71" s="22"/>
     </row>
-    <row r="72" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A72" s="29">
         <v>41883</v>
       </c>
@@ -10207,7 +10214,7 @@
       <c r="AA72" s="22"/>
       <c r="AB72" s="22"/>
     </row>
-    <row r="73" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A73" s="28">
         <v>41852</v>
       </c>
@@ -10252,7 +10259,7 @@
       <c r="AA73" s="22"/>
       <c r="AB73" s="22"/>
     </row>
-    <row r="74" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A74" s="26"/>
       <c r="B74" s="27"/>
       <c r="C74" s="22"/>
@@ -10281,7 +10288,7 @@
       <c r="AA74" s="22"/>
       <c r="AB74" s="22"/>
     </row>
-    <row r="75" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A75" s="55"/>
       <c r="B75" s="55"/>
       <c r="C75" s="22"/>
@@ -10311,7 +10318,7 @@
       <c r="AA75" s="22"/>
       <c r="AB75" s="22"/>
     </row>
-    <row r="76" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A76" s="55"/>
       <c r="B76" s="55"/>
       <c r="C76" s="22"/>
@@ -10341,7 +10348,7 @@
       <c r="AA76" s="22"/>
       <c r="AB76" s="22"/>
     </row>
-    <row r="77" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A77" s="55"/>
       <c r="B77" s="55"/>
       <c r="C77" s="22"/>
@@ -10371,7 +10378,7 @@
       <c r="AA77" s="22"/>
       <c r="AB77" s="22"/>
     </row>
-    <row r="78" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A78" s="55"/>
       <c r="B78" s="55"/>
       <c r="C78" s="22"/>
@@ -10401,251 +10408,251 @@
       <c r="AA78" s="22"/>
       <c r="AB78" s="22"/>
     </row>
-    <row r="79" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
     </row>
-    <row r="80" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="1"/>
       <c r="B115" s="1"/>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="1"/>
       <c r="B116" s="1"/>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C122" s="2"/>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C123" s="2"/>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C124" s="2"/>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C125" s="2"/>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C126" s="2"/>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C127" s="2"/>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C128" s="2"/>
     </row>
-    <row r="129" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="129" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C129" s="2"/>
     </row>
-    <row r="130" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="130" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C130" s="2"/>
     </row>
-    <row r="131" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="131" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C131" s="2"/>
     </row>
-    <row r="132" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="132" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C132" s="2"/>
     </row>
-    <row r="133" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="133" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C133" s="2"/>
     </row>
-    <row r="134" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="134" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C134" s="2"/>
     </row>
-    <row r="135" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="135" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C135" s="2"/>
     </row>
-    <row r="136" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="136" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C136" s="2"/>
     </row>
-    <row r="137" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="137" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C137" s="2"/>
     </row>
-    <row r="138" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="138" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C138" s="2"/>
     </row>
-    <row r="139" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="139" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C139" s="2"/>
     </row>
-    <row r="140" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="140" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C140" s="2"/>
     </row>
-    <row r="141" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="141" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C141" s="2"/>
     </row>
-    <row r="142" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="142" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C142" s="2"/>
     </row>
-    <row r="143" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="143" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C143" s="2"/>
     </row>
-    <row r="144" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="144" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C144" s="2"/>
     </row>
-    <row r="145" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="145" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C145" s="2"/>
     </row>
-    <row r="146" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="146" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C146" s="2"/>
     </row>
   </sheetData>
@@ -10681,25 +10688,25 @@
       <selection activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" hidden="1" customWidth="1"/>
     <col min="3" max="6" width="12" customWidth="1"/>
     <col min="8" max="8" width="0" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="29.5" customWidth="1"/>
-    <col min="10" max="10" width="21.83203125" customWidth="1"/>
-    <col min="11" max="11" width="14.33203125" customWidth="1"/>
-    <col min="12" max="12" width="30.5" customWidth="1"/>
-    <col min="13" max="13" width="11.83203125" customWidth="1"/>
-    <col min="14" max="14" width="9.1640625" customWidth="1"/>
-    <col min="15" max="15" width="28.33203125" customWidth="1"/>
-    <col min="16" max="16" width="17.5" customWidth="1"/>
-    <col min="17" max="17" width="14.33203125" customWidth="1"/>
-    <col min="18" max="18" width="12.6640625" customWidth="1"/>
+    <col min="9" max="9" width="29.42578125" customWidth="1"/>
+    <col min="10" max="10" width="21.85546875" customWidth="1"/>
+    <col min="11" max="11" width="14.28515625" customWidth="1"/>
+    <col min="12" max="12" width="30.42578125" customWidth="1"/>
+    <col min="13" max="13" width="11.85546875" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" customWidth="1"/>
+    <col min="15" max="15" width="28.28515625" customWidth="1"/>
+    <col min="16" max="16" width="17.42578125" customWidth="1"/>
+    <col min="17" max="17" width="14.28515625" customWidth="1"/>
+    <col min="18" max="18" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="32" t="s">
         <v>1210</v>
       </c>
@@ -10729,7 +10736,7 @@
       <c r="AA1" s="22"/>
       <c r="AB1" s="22"/>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>0</v>
       </c>
@@ -10779,7 +10786,7 @@
       <c r="AA2" s="22"/>
       <c r="AB2" s="22"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="28">
         <v>43983</v>
       </c>
@@ -10828,7 +10835,7 @@
       <c r="AA3" s="22"/>
       <c r="AB3" s="22"/>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="29">
         <v>43952</v>
       </c>
@@ -10881,7 +10888,7 @@
       <c r="AA4" s="22"/>
       <c r="AB4" s="22"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="28">
         <v>43922</v>
       </c>
@@ -10935,7 +10942,7 @@
       <c r="AA5" s="22"/>
       <c r="AB5" s="22"/>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="29">
         <v>43891</v>
       </c>
@@ -10989,7 +10996,7 @@
       <c r="AA6" s="22"/>
       <c r="AB6" s="22"/>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="28">
         <v>43862</v>
       </c>
@@ -11039,7 +11046,7 @@
       <c r="AA7" s="22"/>
       <c r="AB7" s="22"/>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" s="29">
         <v>43831</v>
       </c>
@@ -11089,7 +11096,7 @@
       <c r="AA8" s="22"/>
       <c r="AB8" s="22"/>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" s="28">
         <v>43800</v>
       </c>
@@ -11134,7 +11141,7 @@
       <c r="AA9" s="22"/>
       <c r="AB9" s="22"/>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" s="29">
         <v>43770</v>
       </c>
@@ -11183,7 +11190,7 @@
       <c r="AA10" s="22"/>
       <c r="AB10" s="22"/>
     </row>
-    <row r="11" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="28">
         <v>43739</v>
       </c>
@@ -11240,7 +11247,7 @@
       <c r="AA11" s="22"/>
       <c r="AB11" s="22"/>
     </row>
-    <row r="12" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="29">
         <v>43709</v>
       </c>
@@ -11297,7 +11304,7 @@
       <c r="AA12" s="22"/>
       <c r="AB12" s="22"/>
     </row>
-    <row r="13" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="28">
         <v>43678</v>
       </c>
@@ -11354,7 +11361,7 @@
       <c r="AA13" s="22"/>
       <c r="AB13" s="22"/>
     </row>
-    <row r="14" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="29">
         <v>43647</v>
       </c>
@@ -11411,7 +11418,7 @@
       <c r="AA14" s="22"/>
       <c r="AB14" s="22"/>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15" s="28">
         <v>43617</v>
       </c>
@@ -11460,7 +11467,7 @@
       <c r="AA15" s="22"/>
       <c r="AB15" s="22"/>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16" s="29">
         <v>43586</v>
       </c>
@@ -11514,7 +11521,7 @@
       <c r="AA16" s="22"/>
       <c r="AB16" s="22"/>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17" s="28">
         <v>43556</v>
       </c>
@@ -11559,7 +11566,7 @@
       <c r="AA17" s="22"/>
       <c r="AB17" s="22"/>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18" s="29">
         <v>43525</v>
       </c>
@@ -11606,7 +11613,7 @@
       <c r="AA18" s="22"/>
       <c r="AB18" s="22"/>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19" s="28">
         <v>43497</v>
       </c>
@@ -11657,7 +11664,7 @@
       <c r="AA19" s="22"/>
       <c r="AB19" s="22"/>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20" s="29">
         <v>43466</v>
       </c>
@@ -11712,7 +11719,7 @@
       <c r="AA20" s="22"/>
       <c r="AB20" s="22"/>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21" s="28">
         <v>43435</v>
       </c>
@@ -11768,7 +11775,7 @@
       <c r="AA21" s="22"/>
       <c r="AB21" s="22"/>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22" s="29">
         <v>43405</v>
       </c>
@@ -11824,7 +11831,7 @@
       <c r="AA22" s="22"/>
       <c r="AB22" s="22"/>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A23" s="28">
         <v>43374</v>
       </c>
@@ -11879,7 +11886,7 @@
       <c r="AA23" s="22"/>
       <c r="AB23" s="22"/>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A24" s="29">
         <v>43344</v>
       </c>
@@ -11921,7 +11928,7 @@
       <c r="AA24" s="22"/>
       <c r="AB24" s="22"/>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A25" s="28">
         <v>43313</v>
       </c>
@@ -11968,7 +11975,7 @@
       <c r="AA25" s="22"/>
       <c r="AB25" s="22"/>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A26" s="29">
         <v>43282</v>
       </c>
@@ -12017,7 +12024,7 @@
       <c r="AA26" s="22"/>
       <c r="AB26" s="22"/>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A27" s="28">
         <v>43252</v>
       </c>
@@ -12066,7 +12073,7 @@
       <c r="AA27" s="22"/>
       <c r="AB27" s="22"/>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A28" s="29">
         <v>43221</v>
       </c>
@@ -12111,7 +12118,7 @@
       <c r="AA28" s="22"/>
       <c r="AB28" s="22"/>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A29" s="28">
         <v>43191</v>
       </c>
@@ -12170,7 +12177,7 @@
       <c r="AA29" s="22"/>
       <c r="AB29" s="22"/>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A30" s="29">
         <v>43160</v>
       </c>
@@ -12229,7 +12236,7 @@
       <c r="AA30" s="22"/>
       <c r="AB30" s="22"/>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A31" s="28">
         <v>43132</v>
       </c>
@@ -12288,7 +12295,7 @@
       <c r="AA31" s="22"/>
       <c r="AB31" s="22"/>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A32" s="29">
         <v>43101</v>
       </c>
@@ -12347,7 +12354,7 @@
       <c r="AA32" s="22"/>
       <c r="AB32" s="22"/>
     </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A33" s="28">
         <v>43070</v>
       </c>
@@ -12406,7 +12413,7 @@
       <c r="AA33" s="22"/>
       <c r="AB33" s="22"/>
     </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A34" s="29">
         <v>43040</v>
       </c>
@@ -12451,7 +12458,7 @@
       <c r="AA34" s="22"/>
       <c r="AB34" s="22"/>
     </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A35" s="28">
         <v>43009</v>
       </c>
@@ -12498,7 +12505,7 @@
       <c r="AA35" s="22"/>
       <c r="AB35" s="22"/>
     </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A36" s="29">
         <v>42979</v>
       </c>
@@ -12545,7 +12552,7 @@
       <c r="AA36" s="22"/>
       <c r="AB36" s="22"/>
     </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A37" s="28">
         <v>42948</v>
       </c>
@@ -12592,7 +12599,7 @@
       <c r="AA37" s="22"/>
       <c r="AB37" s="22"/>
     </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A38" s="29">
         <v>42917</v>
       </c>
@@ -12639,7 +12646,7 @@
       <c r="AA38" s="22"/>
       <c r="AB38" s="22"/>
     </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A39" s="28">
         <v>42887</v>
       </c>
@@ -12686,7 +12693,7 @@
       <c r="AA39" s="22"/>
       <c r="AB39" s="22"/>
     </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A40" s="29">
         <v>42856</v>
       </c>
@@ -12733,7 +12740,7 @@
       <c r="AA40" s="22"/>
       <c r="AB40" s="22"/>
     </row>
-    <row r="41" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A41" s="28">
         <v>42826</v>
       </c>
@@ -12778,7 +12785,7 @@
       <c r="AA41" s="22"/>
       <c r="AB41" s="22"/>
     </row>
-    <row r="42" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A42" s="29">
         <v>42795</v>
       </c>
@@ -12825,7 +12832,7 @@
       <c r="AA42" s="22"/>
       <c r="AB42" s="22"/>
     </row>
-    <row r="43" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A43" s="28">
         <v>42767</v>
       </c>
@@ -12870,7 +12877,7 @@
       <c r="AA43" s="22"/>
       <c r="AB43" s="22"/>
     </row>
-    <row r="44" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A44" s="29">
         <v>42736</v>
       </c>
@@ -12915,7 +12922,7 @@
       <c r="AA44" s="22"/>
       <c r="AB44" s="22"/>
     </row>
-    <row r="45" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A45" s="28">
         <v>42705</v>
       </c>
@@ -12960,7 +12967,7 @@
       <c r="AA45" s="22"/>
       <c r="AB45" s="22"/>
     </row>
-    <row r="46" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A46" s="29">
         <v>42675</v>
       </c>
@@ -13005,7 +13012,7 @@
       <c r="AA46" s="22"/>
       <c r="AB46" s="22"/>
     </row>
-    <row r="47" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A47" s="28">
         <v>42644</v>
       </c>
@@ -13050,7 +13057,7 @@
       <c r="AA47" s="22"/>
       <c r="AB47" s="22"/>
     </row>
-    <row r="48" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A48" s="29">
         <v>42614</v>
       </c>
@@ -13095,7 +13102,7 @@
       <c r="AA48" s="22"/>
       <c r="AB48" s="22"/>
     </row>
-    <row r="49" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A49" s="28">
         <v>42583</v>
       </c>
@@ -13140,7 +13147,7 @@
       <c r="AA49" s="22"/>
       <c r="AB49" s="22"/>
     </row>
-    <row r="50" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A50" s="29">
         <v>42552</v>
       </c>
@@ -13185,7 +13192,7 @@
       <c r="AA50" s="22"/>
       <c r="AB50" s="22"/>
     </row>
-    <row r="51" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A51" s="28">
         <v>42522</v>
       </c>
@@ -13230,7 +13237,7 @@
       <c r="AA51" s="22"/>
       <c r="AB51" s="22"/>
     </row>
-    <row r="52" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A52" s="29">
         <v>42491</v>
       </c>
@@ -13275,7 +13282,7 @@
       <c r="AA52" s="22"/>
       <c r="AB52" s="22"/>
     </row>
-    <row r="53" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A53" s="28">
         <v>42461</v>
       </c>
@@ -13320,7 +13327,7 @@
       <c r="AA53" s="22"/>
       <c r="AB53" s="22"/>
     </row>
-    <row r="54" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A54" s="29">
         <v>42430</v>
       </c>
@@ -13365,7 +13372,7 @@
       <c r="AA54" s="22"/>
       <c r="AB54" s="22"/>
     </row>
-    <row r="55" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A55" s="28">
         <v>42401</v>
       </c>
@@ -13410,7 +13417,7 @@
       <c r="AA55" s="22"/>
       <c r="AB55" s="22"/>
     </row>
-    <row r="56" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A56" s="29">
         <v>42370</v>
       </c>
@@ -13455,7 +13462,7 @@
       <c r="AA56" s="22"/>
       <c r="AB56" s="22"/>
     </row>
-    <row r="57" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A57" s="28">
         <v>42339</v>
       </c>
@@ -13500,7 +13507,7 @@
       <c r="AA57" s="22"/>
       <c r="AB57" s="22"/>
     </row>
-    <row r="58" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A58" s="29">
         <v>42309</v>
       </c>
@@ -13545,7 +13552,7 @@
       <c r="AA58" s="22"/>
       <c r="AB58" s="22"/>
     </row>
-    <row r="59" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A59" s="28">
         <v>42278</v>
       </c>
@@ -13590,7 +13597,7 @@
       <c r="AA59" s="22"/>
       <c r="AB59" s="22"/>
     </row>
-    <row r="60" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A60" s="29">
         <v>42248</v>
       </c>
@@ -13635,7 +13642,7 @@
       <c r="AA60" s="22"/>
       <c r="AB60" s="22"/>
     </row>
-    <row r="61" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A61" s="28">
         <v>42217</v>
       </c>
@@ -13680,7 +13687,7 @@
       <c r="AA61" s="22"/>
       <c r="AB61" s="22"/>
     </row>
-    <row r="62" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A62" s="29">
         <v>42186</v>
       </c>
@@ -13725,7 +13732,7 @@
       <c r="AA62" s="22"/>
       <c r="AB62" s="22"/>
     </row>
-    <row r="63" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A63" s="28">
         <v>42156</v>
       </c>
@@ -13770,7 +13777,7 @@
       <c r="AA63" s="22"/>
       <c r="AB63" s="22"/>
     </row>
-    <row r="64" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A64" s="29">
         <v>42125</v>
       </c>
@@ -13815,7 +13822,7 @@
       <c r="AA64" s="22"/>
       <c r="AB64" s="22"/>
     </row>
-    <row r="65" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A65" s="28">
         <v>42095</v>
       </c>
@@ -13860,7 +13867,7 @@
       <c r="AA65" s="22"/>
       <c r="AB65" s="22"/>
     </row>
-    <row r="66" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A66" s="29">
         <v>42064</v>
       </c>
@@ -13905,7 +13912,7 @@
       <c r="AA66" s="22"/>
       <c r="AB66" s="22"/>
     </row>
-    <row r="67" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A67" s="28">
         <v>42036</v>
       </c>
@@ -13950,7 +13957,7 @@
       <c r="AA67" s="22"/>
       <c r="AB67" s="22"/>
     </row>
-    <row r="68" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A68" s="29">
         <v>42005</v>
       </c>
@@ -13995,7 +14002,7 @@
       <c r="AA68" s="22"/>
       <c r="AB68" s="22"/>
     </row>
-    <row r="69" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A69" s="28">
         <v>41974</v>
       </c>
@@ -14040,7 +14047,7 @@
       <c r="AA69" s="22"/>
       <c r="AB69" s="22"/>
     </row>
-    <row r="70" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A70" s="29">
         <v>41944</v>
       </c>
@@ -14085,7 +14092,7 @@
       <c r="AA70" s="22"/>
       <c r="AB70" s="22"/>
     </row>
-    <row r="71" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A71" s="28">
         <v>41913</v>
       </c>
@@ -14130,7 +14137,7 @@
       <c r="AA71" s="22"/>
       <c r="AB71" s="22"/>
     </row>
-    <row r="72" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A72" s="29">
         <v>41883</v>
       </c>
@@ -14175,7 +14182,7 @@
       <c r="AA72" s="22"/>
       <c r="AB72" s="22"/>
     </row>
-    <row r="73" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A73" s="28">
         <v>41852</v>
       </c>
@@ -14220,7 +14227,7 @@
       <c r="AA73" s="22"/>
       <c r="AB73" s="22"/>
     </row>
-    <row r="74" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A74" s="26"/>
       <c r="B74" s="27"/>
       <c r="C74" s="22"/>
@@ -14249,7 +14256,7 @@
       <c r="AA74" s="22"/>
       <c r="AB74" s="22"/>
     </row>
-    <row r="75" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A75" s="55"/>
       <c r="B75" s="55"/>
       <c r="C75" s="22"/>
@@ -14279,7 +14286,7 @@
       <c r="AA75" s="22"/>
       <c r="AB75" s="22"/>
     </row>
-    <row r="76" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A76" s="55"/>
       <c r="B76" s="55"/>
       <c r="C76" s="22"/>
@@ -14309,7 +14316,7 @@
       <c r="AA76" s="22"/>
       <c r="AB76" s="22"/>
     </row>
-    <row r="77" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A77" s="55"/>
       <c r="B77" s="55"/>
       <c r="C77" s="22"/>
@@ -14339,7 +14346,7 @@
       <c r="AA77" s="22"/>
       <c r="AB77" s="22"/>
     </row>
-    <row r="78" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A78" s="55"/>
       <c r="B78" s="55"/>
       <c r="C78" s="22"/>
@@ -14369,251 +14376,251 @@
       <c r="AA78" s="22"/>
       <c r="AB78" s="22"/>
     </row>
-    <row r="79" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
     </row>
-    <row r="80" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="1"/>
       <c r="B115" s="1"/>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="1"/>
       <c r="B116" s="1"/>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C122" s="2"/>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C123" s="2"/>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C124" s="2"/>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C125" s="2"/>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C126" s="2"/>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C127" s="2"/>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C128" s="2"/>
     </row>
-    <row r="129" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="129" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C129" s="2"/>
     </row>
-    <row r="130" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="130" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C130" s="2"/>
     </row>
-    <row r="131" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="131" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C131" s="2"/>
     </row>
-    <row r="132" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="132" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C132" s="2"/>
     </row>
-    <row r="133" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="133" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C133" s="2"/>
     </row>
-    <row r="134" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="134" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C134" s="2"/>
     </row>
-    <row r="135" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="135" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C135" s="2"/>
     </row>
-    <row r="136" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="136" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C136" s="2"/>
     </row>
-    <row r="137" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="137" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C137" s="2"/>
     </row>
-    <row r="138" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="138" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C138" s="2"/>
     </row>
-    <row r="139" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="139" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C139" s="2"/>
     </row>
-    <row r="140" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="140" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C140" s="2"/>
     </row>
-    <row r="141" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="141" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C141" s="2"/>
     </row>
-    <row r="142" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="142" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C142" s="2"/>
     </row>
-    <row r="143" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="143" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C143" s="2"/>
     </row>
-    <row r="144" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="144" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C144" s="2"/>
     </row>
-    <row r="145" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="145" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C145" s="2"/>
     </row>
-    <row r="146" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="146" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C146" s="2"/>
     </row>
   </sheetData>
@@ -14649,12 +14656,12 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.83203125" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>19</v>
       </c>
@@ -14662,7 +14669,7 @@
         <v>1214</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>1645</v>
       </c>
@@ -14670,7 +14677,7 @@
         <v>1209</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>1640</v>
       </c>
@@ -14678,7 +14685,7 @@
         <v>1644</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>1371</v>
       </c>
@@ -14686,7 +14693,7 @@
         <v>1643</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>1641</v>
       </c>
@@ -14694,7 +14701,7 @@
         <v>1642</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>1646</v>
       </c>
@@ -14702,7 +14709,7 @@
         <v>1213</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>1647</v>
       </c>
@@ -14710,7 +14717,7 @@
         <v>1215</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>1208</v>
       </c>
@@ -14736,20 +14743,20 @@
       <selection activeCell="BS1" sqref="BS1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.6640625" customWidth="1"/>
-    <col min="17" max="17" width="12.6640625" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" customWidth="1"/>
+    <col min="17" max="17" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -14943,7 +14950,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="2" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43983</v>
       </c>
@@ -15145,7 +15152,7 @@
         <v>2.7999999999999994E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43952</v>
       </c>
@@ -15347,7 +15354,7 @@
         <v>-9.2470277410832604E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43922</v>
       </c>
@@ -15549,7 +15556,7 @@
         <v>1.6107382550335586E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43891</v>
       </c>
@@ -15751,7 +15758,7 @@
         <v>-0.11520190023752966</v>
       </c>
     </row>
-    <row r="6" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43862</v>
       </c>
@@ -15953,7 +15960,7 @@
         <v>-1.1862396204032962E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43831</v>
       </c>
@@ -16155,7 +16162,7 @@
         <v>-2.4305555555555653E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43800</v>
       </c>
@@ -16357,7 +16364,7 @@
         <v>1.2895662368112687E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43770</v>
       </c>
@@ -16559,7 +16566,7 @@
         <v>-8.1395348837209631E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43739</v>
       </c>
@@ -16761,7 +16768,7 @@
         <v>3.9903264812575584E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>43709</v>
       </c>
@@ -16963,7 +16970,7 @@
         <v>-2.1301775147928963E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>43678</v>
       </c>
@@ -17165,7 +17172,7 @@
         <v>4.7562425683708859E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>43647</v>
       </c>
@@ -17367,7 +17374,7 @@
         <v>-2.5492468134414904E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>43617</v>
       </c>
@@ -17569,7 +17576,7 @@
         <v>2.0094562647754128E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>43586</v>
       </c>
@@ -17771,7 +17778,7 @@
         <v>-2.5345622119815538E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>43556</v>
       </c>
@@ -17973,7 +17980,7 @@
         <v>-2.2988505747125951E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>43525</v>
       </c>
@@ -18175,7 +18182,7 @@
         <v>-2.6845637583892641E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>43497</v>
       </c>
@@ -18377,7 +18384,7 @@
         <v>-1.1173184357541662E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>43466</v>
       </c>
@@ -18579,7 +18586,7 @@
         <v>3.3632286995514977E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>43435</v>
       </c>
@@ -18781,7 +18788,7 @@
         <v>1.2485811577752489E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>43405</v>
       </c>
@@ -18983,7 +18990,7 @@
         <v>-1.1223344556677849E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>43374</v>
       </c>
@@ -19185,7 +19192,7 @@
         <v>-4.4692737430166649E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>43344</v>
       </c>
@@ -19387,7 +19394,7 @@
         <v>-1.7563117453347987E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>43313</v>
       </c>
@@ -19589,7 +19596,7 @@
         <v>1.5607580824971993E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>43282</v>
       </c>
@@ -19791,7 +19798,7 @@
         <v>0.12547051442910928</v>
       </c>
     </row>
-    <row r="26" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>43252</v>
       </c>
@@ -19993,7 +20000,7 @@
         <v>-5.9031877213695495E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>43221</v>
       </c>
@@ -20195,7 +20202,7 @@
         <v>-0.11215932914046108</v>
       </c>
     </row>
-    <row r="28" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>43191</v>
       </c>
@@ -20397,7 +20404,7 @@
         <v>1.7057569296375089E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>43160</v>
       </c>
@@ -20599,7 +20606,7 @@
         <v>1.2958963282937472E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>43132</v>
       </c>
@@ -20801,7 +20808,7 @@
         <v>3.5794183445190191E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>43101</v>
       </c>
@@ -21003,7 +21010,7 @@
         <v>3.1141868512110676E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>43070</v>
       </c>
@@ -21205,7 +21212,7 @@
         <v>5.8608058608058664E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>43040</v>
       </c>
@@ -21407,7 +21414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>43009</v>
       </c>
@@ -21609,7 +21616,7 @@
         <v>-6.0679611650486295E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>42979</v>
       </c>
@@ -21811,7 +21818,7 @@
         <v>7.3349633251834348E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>42948</v>
       </c>
@@ -22013,7 +22020,7 @@
         <v>-8.4848484848485187E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>42917</v>
       </c>
@@ -22215,7 +22222,7 @@
         <v>-8.4134615384615728E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>42887</v>
       </c>
@@ -22417,7 +22424,7 @@
         <v>4.3914680050188275E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>42856</v>
       </c>
@@ -22619,7 +22626,7 @@
         <v>-1.4833127317676156E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>42826</v>
       </c>
@@ -22821,7 +22828,7 @@
         <v>7.436918990703846E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>42795</v>
       </c>
@@ -23023,7 +23030,7 @@
         <v>3.7190082644628163E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>42767</v>
       </c>
@@ -23225,7 +23232,7 @@
         <v>4.6109510086455245E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>42736</v>
       </c>
@@ -23427,7 +23434,7 @@
         <v>1.4430014430015404E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>42705</v>
       </c>
@@ -23629,7 +23636,7 @@
         <v>5.6402439024390266E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>42675</v>
       </c>
@@ -23831,7 +23838,7 @@
         <v>-1.649175412293858E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>42644</v>
       </c>
@@ -24033,7 +24040,7 @@
         <v>8.1037277147487846E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>42614</v>
       </c>
@@ -24235,7 +24242,7 @@
         <v>-5.6574923547400631E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>42583</v>
       </c>
@@ -24437,7 +24444,7 @@
         <v>-9.0909090909090315E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>42552</v>
       </c>
@@ -24639,7 +24646,7 @@
         <v>-1.4925373134328438E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>42522</v>
       </c>
@@ -24841,7 +24848,7 @@
         <v>3.2357473035439129E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>42491</v>
       </c>
@@ -25043,7 +25050,7 @@
         <v>-8.5915492957746406E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>42461</v>
       </c>
@@ -25245,7 +25252,7 @@
         <v>-9.762900976290137E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>42430</v>
       </c>
@@ -25447,7 +25454,7 @@
         <v>6.0650887573964522E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>42401</v>
       </c>
@@ -25649,7 +25656,7 @@
         <v>-8.7976539589443535E-3</v>
       </c>
     </row>
-    <row r="55" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>42370</v>
       </c>
@@ -25851,7 +25858,7 @@
         <v>2.0958083832335415E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>42339</v>
       </c>
@@ -26053,7 +26060,7 @@
         <v>1.0590015128592948E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>42309</v>
       </c>
@@ -26255,7 +26262,7 @@
         <v>3.6050156739811982E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>42278</v>
       </c>
@@ -26457,7 +26464,7 @@
         <v>-3.6253776435045348E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>42248</v>
       </c>
@@ -26659,7 +26666,7 @@
         <v>-2.2156573116691208E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>42217</v>
       </c>
@@ -26861,7 +26868,7 @@
         <v>-4.7819971870604883E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>42186</v>
       </c>
@@ -27063,7 +27070,7 @@
         <v>7.08215297450435E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>42156</v>
       </c>
@@ -27265,7 +27272,7 @@
         <v>1.1461318051575813E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>42125</v>
       </c>
@@ -27467,7 +27474,7 @@
         <v>1.6011644832605577E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>42095</v>
       </c>
@@ -27669,7 +27676,7 @@
         <v>-1.29310344827586E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>42064</v>
       </c>
@@ -27871,7 +27878,7 @@
         <v>1.4577259475218606E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>42036</v>
       </c>
@@ -28073,7 +28080,7 @@
         <v>5.3763440860215138E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>42005</v>
       </c>
@@ -28275,7 +28282,7 @@
         <v>-4.824561403508773E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>41974</v>
       </c>
@@ -28477,7 +28484,7 @@
         <v>-3.1161473087818664E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>41944</v>
       </c>
@@ -28679,7 +28686,7 @@
         <v>-2.4861878453038756E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>41913</v>
       </c>
@@ -28881,7 +28888,7 @@
         <v>-1.3793103448275568E-3</v>
       </c>
     </row>
-    <row r="71" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>41883</v>
       </c>
@@ -29083,7 +29090,7 @@
         <v>-1.4945652173913086E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>41852</v>
       </c>
@@ -29285,7 +29292,7 @@
         <v>2.222222222222224E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>41821</v>
       </c>

</xml_diff>